<commit_message>
Request system completed fully
</commit_message>
<xml_diff>
--- a/public/templates/template_file.xlsx
+++ b/public/templates/template_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Inventory 2081-82 developmentfolder\inventory-backend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797A6B02-F22F-43D8-AAAD-CDC743384F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47D870D-F23B-492D-9C65-BBE7B8C2147D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -666,6 +666,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="10"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="14"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -758,6 +767,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -937,15 +952,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>-57154</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
+      <xdr:colOff>714371</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -960,13 +975,12 @@
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="3093" r="-1"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1790700" cy="666750"/>
+          <a:off x="-57154" y="0"/>
+          <a:ext cx="1847850" cy="666750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1330,46 +1344,46 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="56" t="s">
+      <c r="E7" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="60"/>
-      <c r="H7" s="54" t="s">
+      <c r="G7" s="63"/>
+      <c r="H7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="57" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
       <c r="F8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
@@ -1431,20 +1445,20 @@
       <c r="A16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="58" t="s">
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="I16" s="58"/>
+      <c r="I16" s="61"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1510,12 +1524,12 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
       <c r="I3" s="21" t="s">
         <v>42</v>
       </c>
@@ -1525,10 +1539,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
       <c r="I4" s="23" t="s">
         <v>9</v>
       </c>
@@ -1563,46 +1577,46 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="54" t="s">
+      <c r="G8" s="63"/>
+      <c r="H8" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="57" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
       <c r="F9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
@@ -1705,27 +1719,27 @@
       <c r="A17" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="58" t="s">
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="I17" s="65"/>
+      <c r="I17" s="68"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
       <c r="I18" s="31" t="s">
         <v>37</v>
       </c>
@@ -1734,12 +1748,12 @@
       <c r="A19" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="63" t="s">
+      <c r="D19" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
       <c r="I19" s="31" t="s">
         <v>38</v>
       </c>
@@ -1750,12 +1764,12 @@
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
-      <c r="D20" s="64" t="s">
+      <c r="D20" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="33"/>
       <c r="I20" s="34" t="s">
         <v>39</v>
@@ -1849,13 +1863,13 @@
         <v>54</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
       <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1863,11 +1877,11 @@
         <v>55</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1880,52 +1894,52 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="66" t="s">
+      <c r="H7" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="66"/>
+      <c r="I7" s="69"/>
     </row>
     <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="54" t="s">
+      <c r="G8" s="63"/>
+      <c r="H8" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="57" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
       <c r="F9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
@@ -1967,40 +1981,40 @@
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
       <c r="I13" s="45" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="71"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="73"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="76"/>
       <c r="I14" s="43"/>
     </row>
     <row r="15" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="74"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="76"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="79"/>
       <c r="I15" s="44"/>
     </row>
     <row r="16" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2013,20 +2027,20 @@
       </c>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
-      <c r="D19" s="68" t="s">
+      <c r="D19" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="69" t="s">
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="I19" s="69"/>
+      <c r="I19" s="72"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2070,7 +2084,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E8" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2101,7 +2115,7 @@
       </c>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="42"/>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
@@ -2113,10 +2127,13 @@
     <row r="3" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="15"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
+      <c r="C3" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="42"/>
       <c r="I3" s="37" t="s">
         <v>9</v>
@@ -2127,28 +2144,21 @@
         <v>54</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="D4" s="67" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
       <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>49</v>
@@ -2158,132 +2168,139 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="66" t="s">
+      <c r="H7" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="66"/>
+      <c r="I7" s="69"/>
     </row>
     <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="54" t="s">
+      <c r="G8" s="63"/>
+      <c r="H8" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="57" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
       <c r="F9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-    </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+    </row>
+    <row r="10" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>1</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+    </row>
+    <row r="11" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>2</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="89"/>
+    </row>
+    <row r="12" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>3</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
     </row>
     <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
       <c r="I13" s="45" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="77"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="83"/>
-    </row>
-    <row r="15" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="80"/>
-      <c r="B15" s="81"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="84"/>
-    </row>
-    <row r="16" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="86"/>
+    </row>
+    <row r="15" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="83"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="87"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="56"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
@@ -2346,11 +2363,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="A14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="A13:H13"/>
-    <mergeCell ref="D4:H5"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
@@ -2361,7 +2377,7 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
   </mergeCells>
-  <pageMargins left="0.47" right="0.59" top="0.46" bottom="0.2" header="0.46" footer="0.2"/>
+  <pageMargins left="0.47" right="0.59" top="0.42" bottom="0.17" header="0.46" footer="0.2"/>
   <pageSetup paperSize="9" scale="99" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Bin card system almost complete.Now generate by issue date left
</commit_message>
<xml_diff>
--- a/public/templates/template_file.xlsx
+++ b/public/templates/template_file.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Inventory 2081-82 developmentfolder\inventory-backend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6924FA-CF0E-4EC7-AD3A-517DEE9F0AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE599D35-744F-4619-8534-1A40742A0394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Request Template" sheetId="21" r:id="rId1"/>
     <sheet name="RRFP Template" sheetId="22" r:id="rId2"/>
     <sheet name="RRLP Template" sheetId="23" r:id="rId3"/>
+    <sheet name="Stock Card Template" sheetId="24" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
   <si>
     <t>U/M</t>
   </si>
@@ -265,6 +266,105 @@
   </si>
   <si>
     <t>NPR</t>
+  </si>
+  <si>
+    <t>Form no. GrSD/STK01</t>
+  </si>
+  <si>
+    <t>Revision: 01 (October 2022)</t>
+  </si>
+  <si>
+    <t>Stock Card</t>
+  </si>
+  <si>
+    <t>Card No:</t>
+  </si>
+  <si>
+    <t>NAC Code:</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Type of Stock:</t>
+  </si>
+  <si>
+    <t>Location:</t>
+  </si>
+  <si>
+    <t>Nomenclature:</t>
+  </si>
+  <si>
+    <t>Part No.:</t>
+  </si>
+  <si>
+    <t>Alternate P/N:</t>
+  </si>
+  <si>
+    <t>Applicable Fleet:</t>
+  </si>
+  <si>
+    <t>Stock Level</t>
+  </si>
+  <si>
+    <t>Max:</t>
+  </si>
+  <si>
+    <t>Min:</t>
+  </si>
+  <si>
+    <t>Order Limit:</t>
+  </si>
+  <si>
+    <t>Order Qty:</t>
+  </si>
+  <si>
+    <t>Check/Reviewed By:</t>
+  </si>
+  <si>
+    <t>Recommended By:</t>
+  </si>
+  <si>
+    <t>Signature:</t>
+  </si>
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>Staff ID:</t>
+  </si>
+  <si>
+    <t>Designation:</t>
+  </si>
+  <si>
+    <t>Stock Level Status/Record</t>
+  </si>
+  <si>
+    <t>Receipt</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>Balance Qty.</t>
+  </si>
+  <si>
+    <t>Signature</t>
+  </si>
+  <si>
+    <t>GSE No.</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Ref.</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Qty.</t>
   </si>
 </sst>
 </file>
@@ -275,7 +375,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +533,46 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -454,7 +594,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -613,12 +753,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -983,6 +1141,136 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1028,16 +1316,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1047,23 +1332,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="40"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="40"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="40"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="40"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1122,6 +1410,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1631,52 +1949,52 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="141" t="s">
+      <c r="H7" s="185" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="141"/>
+      <c r="I7" s="185"/>
     </row>
     <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="142" t="s">
+      <c r="A8" s="186" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="144" t="s">
+      <c r="B8" s="188" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="142" t="s">
+      <c r="C8" s="186" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="142" t="s">
+      <c r="D8" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="142" t="s">
+      <c r="E8" s="186" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="146" t="s">
+      <c r="F8" s="190" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="146"/>
-      <c r="H8" s="144" t="s">
+      <c r="G8" s="190"/>
+      <c r="H8" s="188" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="144" t="s">
+      <c r="I8" s="188" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
-      <c r="B9" s="145"/>
-      <c r="C9" s="143"/>
-      <c r="D9" s="143"/>
-      <c r="E9" s="143"/>
+      <c r="A9" s="187"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
       <c r="F9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="145"/>
-      <c r="I9" s="145"/>
+      <c r="H9" s="189"/>
+      <c r="I9" s="189"/>
     </row>
     <row r="10" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
@@ -1718,41 +2036,41 @@
       <c r="I12" s="30"/>
     </row>
     <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="140" t="s">
+      <c r="A13" s="184" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="140"/>
-      <c r="C13" s="140"/>
-      <c r="D13" s="140"/>
-      <c r="E13" s="140"/>
-      <c r="F13" s="140"/>
-      <c r="G13" s="140"/>
-      <c r="H13" s="140"/>
+      <c r="B13" s="184"/>
+      <c r="C13" s="184"/>
+      <c r="D13" s="184"/>
+      <c r="E13" s="184"/>
+      <c r="F13" s="184"/>
+      <c r="G13" s="184"/>
+      <c r="H13" s="184"/>
       <c r="I13" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="132"/>
-      <c r="B14" s="133"/>
-      <c r="C14" s="133"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="133"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="133"/>
-      <c r="H14" s="134"/>
-      <c r="I14" s="138"/>
+      <c r="A14" s="176"/>
+      <c r="B14" s="177"/>
+      <c r="C14" s="177"/>
+      <c r="D14" s="177"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="177"/>
+      <c r="G14" s="177"/>
+      <c r="H14" s="178"/>
+      <c r="I14" s="182"/>
     </row>
     <row r="15" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="135"/>
-      <c r="B15" s="136"/>
-      <c r="C15" s="136"/>
-      <c r="D15" s="136"/>
-      <c r="E15" s="136"/>
-      <c r="F15" s="136"/>
-      <c r="G15" s="136"/>
-      <c r="H15" s="137"/>
-      <c r="I15" s="139"/>
+      <c r="A15" s="179"/>
+      <c r="B15" s="180"/>
+      <c r="C15" s="180"/>
+      <c r="D15" s="180"/>
+      <c r="E15" s="180"/>
+      <c r="F15" s="180"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="181"/>
+      <c r="I15" s="183"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
@@ -1850,7 +2168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82553E5E-DF17-47D3-A9C3-FA8D94FB7CC0}">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -1874,48 +2192,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="202" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
-      <c r="I1" s="160"/>
-      <c r="J1" s="160"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="203"/>
+      <c r="I1" s="203"/>
+      <c r="J1" s="203"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="208" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
-      <c r="J2" s="165"/>
+      <c r="B2" s="209"/>
+      <c r="C2" s="209"/>
+      <c r="D2" s="209"/>
+      <c r="E2" s="209"/>
+      <c r="F2" s="209"/>
+      <c r="G2" s="209"/>
+      <c r="H2" s="209"/>
+      <c r="I2" s="209"/>
+      <c r="J2" s="209"/>
       <c r="K2" s="38"/>
       <c r="L2" s="72"/>
     </row>
     <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="210" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="167"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-      <c r="I3" s="167"/>
-      <c r="J3" s="167"/>
+      <c r="B3" s="211"/>
+      <c r="C3" s="211"/>
+      <c r="D3" s="211"/>
+      <c r="E3" s="211"/>
+      <c r="F3" s="211"/>
+      <c r="G3" s="211"/>
+      <c r="H3" s="211"/>
+      <c r="I3" s="211"/>
+      <c r="J3" s="211"/>
       <c r="K3" s="73"/>
       <c r="L3" s="127" t="s">
         <v>73</v>
@@ -2229,29 +2547,29 @@
       <c r="K23" s="34"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="157" t="s">
+      <c r="A24" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="152"/>
+      <c r="B24" s="195"/>
       <c r="C24" s="44"/>
       <c r="D24" s="21"/>
-      <c r="J24" s="153" t="s">
+      <c r="J24" s="196" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="151"/>
-      <c r="L24" s="152"/>
+      <c r="K24" s="194"/>
+      <c r="L24" s="195"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="153" t="s">
+      <c r="A25" s="196" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="152"/>
+      <c r="B25" s="195"/>
       <c r="C25" s="52"/>
       <c r="D25" s="39"/>
-      <c r="E25" s="153" t="s">
+      <c r="E25" s="196" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="152"/>
+      <c r="F25" s="195"/>
       <c r="G25" s="44"/>
       <c r="H25" s="51" t="s">
         <v>75</v>
@@ -2259,40 +2577,40 @@
       <c r="J25" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="153" t="s">
+      <c r="K25" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="L25" s="152"/>
-      <c r="M25" s="149"/>
-      <c r="N25" s="150"/>
-      <c r="O25" s="149"/>
-      <c r="P25" s="150"/>
-      <c r="Q25" s="150"/>
+      <c r="L25" s="195"/>
+      <c r="M25" s="191"/>
+      <c r="N25" s="192"/>
+      <c r="O25" s="191"/>
+      <c r="P25" s="192"/>
+      <c r="Q25" s="192"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="156" t="s">
+      <c r="A26" s="201" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="152"/>
+      <c r="B26" s="195"/>
       <c r="C26" s="49"/>
       <c r="D26" s="48"/>
-      <c r="E26" s="157" t="s">
+      <c r="E26" s="205" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="152"/>
+      <c r="F26" s="195"/>
       <c r="G26" s="47">
         <v>1</v>
       </c>
       <c r="H26" s="46"/>
       <c r="J26" s="45"/>
-      <c r="K26" s="162"/>
-      <c r="L26" s="163"/>
+      <c r="K26" s="206"/>
+      <c r="L26" s="207"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="153" t="s">
+      <c r="A27" s="196" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="152"/>
+      <c r="B27" s="195"/>
       <c r="C27" s="43"/>
       <c r="D27" s="39"/>
       <c r="E27" s="1"/>
@@ -2300,8 +2618,8 @@
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
       <c r="J27" s="42"/>
-      <c r="K27" s="154"/>
-      <c r="L27" s="155"/>
+      <c r="K27" s="197"/>
+      <c r="L27" s="198"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
@@ -2322,72 +2640,72 @@
       <c r="I29" s="32"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="161" t="s">
+      <c r="A30" s="204" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="151"/>
-      <c r="C30" s="152"/>
-      <c r="D30" s="158" t="s">
+      <c r="B30" s="194"/>
+      <c r="C30" s="195"/>
+      <c r="D30" s="200" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="151"/>
-      <c r="F30" s="151"/>
-      <c r="G30" s="152"/>
-      <c r="H30" s="158" t="s">
+      <c r="E30" s="194"/>
+      <c r="F30" s="194"/>
+      <c r="G30" s="195"/>
+      <c r="H30" s="200" t="s">
         <v>30</v>
       </c>
-      <c r="I30" s="158"/>
-      <c r="J30" s="158"/>
+      <c r="I30" s="200"/>
+      <c r="J30" s="200"/>
       <c r="K30" s="50" t="s">
         <v>29</v>
       </c>
       <c r="L30" s="128"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="147"/>
-      <c r="B31" s="151"/>
-      <c r="C31" s="152"/>
-      <c r="D31" s="147"/>
-      <c r="E31" s="151"/>
-      <c r="F31" s="151"/>
-      <c r="G31" s="152"/>
-      <c r="H31" s="147"/>
-      <c r="I31" s="147"/>
-      <c r="J31" s="147"/>
+      <c r="A31" s="193"/>
+      <c r="B31" s="194"/>
+      <c r="C31" s="195"/>
+      <c r="D31" s="193"/>
+      <c r="E31" s="194"/>
+      <c r="F31" s="194"/>
+      <c r="G31" s="195"/>
+      <c r="H31" s="193"/>
+      <c r="I31" s="193"/>
+      <c r="J31" s="193"/>
       <c r="K31" s="129"/>
       <c r="L31" s="124"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="147"/>
-      <c r="B32" s="151"/>
-      <c r="C32" s="152"/>
-      <c r="D32" s="147"/>
-      <c r="E32" s="151"/>
-      <c r="F32" s="151"/>
-      <c r="G32" s="152"/>
-      <c r="H32" s="147"/>
-      <c r="I32" s="147"/>
-      <c r="J32" s="147"/>
+      <c r="A32" s="193"/>
+      <c r="B32" s="194"/>
+      <c r="C32" s="195"/>
+      <c r="D32" s="193"/>
+      <c r="E32" s="194"/>
+      <c r="F32" s="194"/>
+      <c r="G32" s="195"/>
+      <c r="H32" s="193"/>
+      <c r="I32" s="193"/>
+      <c r="J32" s="193"/>
       <c r="K32" s="129"/>
       <c r="L32" s="124"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="147" t="s">
+      <c r="A33" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="151"/>
-      <c r="C33" s="152"/>
-      <c r="D33" s="147" t="s">
+      <c r="B33" s="194"/>
+      <c r="C33" s="195"/>
+      <c r="D33" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="151"/>
-      <c r="F33" s="151"/>
-      <c r="G33" s="152"/>
-      <c r="H33" s="147" t="s">
+      <c r="E33" s="194"/>
+      <c r="F33" s="194"/>
+      <c r="G33" s="195"/>
+      <c r="H33" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="I33" s="147"/>
-      <c r="J33" s="148"/>
+      <c r="I33" s="193"/>
+      <c r="J33" s="199"/>
       <c r="K33" s="129" t="s">
         <v>28</v>
       </c>
@@ -2395,6 +2713,9 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="A30:C30"/>
@@ -2404,23 +2725,20 @@
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="D31:G31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="H33:J33"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
     <mergeCell ref="O25:Q25"/>
     <mergeCell ref="D32:G32"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="M25:N25"/>
     <mergeCell ref="K27:L27"/>
-    <mergeCell ref="D33:G33"/>
     <mergeCell ref="H32:J32"/>
   </mergeCells>
   <pageMargins left="0.23" right="0.17" top="0.64" bottom="0.17" header="0.38" footer="0.17"/>
@@ -2456,45 +2774,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="212" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="169"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
-      <c r="G1" s="169"/>
-      <c r="H1" s="169"/>
-      <c r="I1" s="169"/>
-      <c r="J1" s="169"/>
+      <c r="B1" s="213"/>
+      <c r="C1" s="214"/>
+      <c r="D1" s="213"/>
+      <c r="E1" s="213"/>
+      <c r="F1" s="213"/>
+      <c r="G1" s="213"/>
+      <c r="H1" s="213"/>
+      <c r="I1" s="213"/>
+      <c r="J1" s="213"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="173" t="s">
+      <c r="A2" s="217" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="174"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
-      <c r="I2" s="174"/>
-      <c r="J2" s="174"/>
+      <c r="B2" s="218"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218"/>
+      <c r="G2" s="218"/>
+      <c r="H2" s="218"/>
+      <c r="I2" s="218"/>
+      <c r="J2" s="218"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="177" t="s">
+      <c r="A3" s="221" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="178"/>
-      <c r="C3" s="178"/>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="178"/>
-      <c r="H3" s="178"/>
-      <c r="I3" s="178"/>
+      <c r="B3" s="222"/>
+      <c r="C3" s="222"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="222"/>
+      <c r="H3" s="222"/>
+      <c r="I3" s="222"/>
       <c r="J3" s="127" t="s">
         <v>74</v>
       </c>
@@ -2760,12 +3078,12 @@
       <c r="M21" s="108"/>
     </row>
     <row r="22" spans="1:13" s="99" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="179" t="s">
+      <c r="A22" s="223" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="151"/>
-      <c r="C22" s="151"/>
-      <c r="D22" s="152"/>
+      <c r="B22" s="194"/>
+      <c r="C22" s="194"/>
+      <c r="D22" s="195"/>
       <c r="E22" s="106"/>
       <c r="F22" s="43"/>
       <c r="G22" s="105">
@@ -2797,37 +3115,37 @@
       <c r="K23" s="100"/>
     </row>
     <row r="24" spans="1:13" s="99" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="153" t="s">
+      <c r="A24" s="196" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="152"/>
-      <c r="C24" s="172"/>
-      <c r="D24" s="151"/>
-      <c r="E24" s="152"/>
+      <c r="B24" s="195"/>
+      <c r="C24" s="216"/>
+      <c r="D24" s="194"/>
+      <c r="E24" s="195"/>
       <c r="F24" s="38"/>
       <c r="G24" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="171"/>
-      <c r="I24" s="151"/>
-      <c r="J24" s="152"/>
+      <c r="H24" s="215"/>
+      <c r="I24" s="194"/>
+      <c r="J24" s="195"/>
       <c r="K24" s="100"/>
     </row>
     <row r="25" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="153" t="s">
+      <c r="A25" s="196" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="152"/>
-      <c r="C25" s="172"/>
-      <c r="D25" s="151"/>
-      <c r="E25" s="152"/>
+      <c r="B25" s="195"/>
+      <c r="C25" s="216"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
       <c r="F25" s="38"/>
       <c r="G25" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="H25" s="176"/>
-      <c r="I25" s="151"/>
-      <c r="J25" s="152"/>
+      <c r="H25" s="220"/>
+      <c r="I25" s="194"/>
+      <c r="J25" s="195"/>
     </row>
     <row r="26" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="95"/>
@@ -2843,72 +3161,72 @@
       <c r="K26" s="92"/>
     </row>
     <row r="27" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="147" t="s">
+      <c r="A27" s="193" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="152"/>
-      <c r="C27" s="158" t="s">
+      <c r="B27" s="195"/>
+      <c r="C27" s="200" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="152"/>
+      <c r="D27" s="195"/>
       <c r="E27" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
       <c r="H27" s="94"/>
-      <c r="I27" s="147" t="s">
+      <c r="I27" s="193" t="s">
         <v>29</v>
       </c>
-      <c r="J27" s="152"/>
+      <c r="J27" s="195"/>
       <c r="K27" s="92"/>
       <c r="M27" s="93"/>
     </row>
     <row r="28" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="147"/>
-      <c r="B28" s="152"/>
-      <c r="C28" s="147"/>
-      <c r="D28" s="152"/>
-      <c r="E28" s="147"/>
-      <c r="F28" s="151"/>
-      <c r="G28" s="151"/>
-      <c r="H28" s="152"/>
-      <c r="I28" s="147"/>
-      <c r="J28" s="152"/>
+      <c r="A28" s="193"/>
+      <c r="B28" s="195"/>
+      <c r="C28" s="193"/>
+      <c r="D28" s="195"/>
+      <c r="E28" s="193"/>
+      <c r="F28" s="194"/>
+      <c r="G28" s="194"/>
+      <c r="H28" s="195"/>
+      <c r="I28" s="193"/>
+      <c r="J28" s="195"/>
       <c r="K28" s="92"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="147"/>
-      <c r="B29" s="152"/>
-      <c r="C29" s="147"/>
-      <c r="D29" s="152"/>
-      <c r="E29" s="147"/>
-      <c r="F29" s="151"/>
-      <c r="G29" s="151"/>
-      <c r="H29" s="152"/>
-      <c r="I29" s="147"/>
-      <c r="J29" s="152"/>
+      <c r="A29" s="193"/>
+      <c r="B29" s="195"/>
+      <c r="C29" s="193"/>
+      <c r="D29" s="195"/>
+      <c r="E29" s="193"/>
+      <c r="F29" s="194"/>
+      <c r="G29" s="194"/>
+      <c r="H29" s="195"/>
+      <c r="I29" s="193"/>
+      <c r="J29" s="195"/>
       <c r="L29" s="90"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="147" t="s">
+      <c r="A30" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="152"/>
-      <c r="C30" s="147" t="s">
+      <c r="B30" s="195"/>
+      <c r="C30" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="152"/>
-      <c r="E30" s="147" t="s">
+      <c r="D30" s="195"/>
+      <c r="E30" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="151"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="152"/>
-      <c r="I30" s="147" t="s">
+      <c r="F30" s="194"/>
+      <c r="G30" s="194"/>
+      <c r="H30" s="195"/>
+      <c r="I30" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="152"/>
+      <c r="J30" s="195"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
@@ -2965,8 +3283,8 @@
       <c r="D35" s="77"/>
       <c r="E35" s="82"/>
       <c r="F35" s="82"/>
-      <c r="G35" s="180"/>
-      <c r="H35" s="181"/>
+      <c r="G35" s="224"/>
+      <c r="H35" s="225"/>
       <c r="I35" s="82"/>
       <c r="J35" s="81"/>
     </row>
@@ -3015,4 +3333,1353 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7879FCE9-C911-4935-AAFA-B091B117DCC8}">
+  <dimension ref="A1:K96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" style="136" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="136" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" style="136" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="136" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="136" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" style="136" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" style="136" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="136" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="136" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="136" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="136" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="136"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="132"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="135" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="137"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="139" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="12" x14ac:dyDescent="0.2">
+      <c r="A3" s="140"/>
+      <c r="F3" s="141" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="142"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="143"/>
+    </row>
+    <row r="4" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A4" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="144" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="145"/>
+      <c r="K4" s="146"/>
+    </row>
+    <row r="5" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A5" s="147" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="148"/>
+      <c r="C5" s="148"/>
+      <c r="D5" s="148"/>
+      <c r="E5" s="148"/>
+      <c r="F5" s="148"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="150" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="148"/>
+      <c r="K5" s="146"/>
+    </row>
+    <row r="6" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A6" s="147" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="148"/>
+      <c r="C6" s="148"/>
+      <c r="D6" s="148"/>
+      <c r="E6" s="148"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="150" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="148"/>
+      <c r="K6" s="146"/>
+    </row>
+    <row r="7" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A7" s="147" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="148"/>
+      <c r="C7" s="148"/>
+      <c r="D7" s="148"/>
+      <c r="E7" s="148"/>
+      <c r="F7" s="148"/>
+      <c r="G7" s="148"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
+      <c r="K7" s="152"/>
+    </row>
+    <row r="8" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A8" s="147" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="148"/>
+      <c r="C8" s="148"/>
+      <c r="D8" s="148"/>
+      <c r="E8" s="148"/>
+      <c r="F8" s="148"/>
+      <c r="G8" s="148"/>
+      <c r="H8" s="148"/>
+      <c r="I8" s="149"/>
+      <c r="J8" s="149"/>
+      <c r="K8" s="152"/>
+    </row>
+    <row r="9" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A9" s="147" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="148"/>
+      <c r="C9" s="148"/>
+      <c r="D9" s="148"/>
+      <c r="E9" s="148"/>
+      <c r="F9" s="148"/>
+      <c r="G9" s="148"/>
+      <c r="H9" s="148"/>
+      <c r="I9" s="149"/>
+      <c r="J9" s="149"/>
+      <c r="K9" s="152"/>
+    </row>
+    <row r="10" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A10" s="147" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="148"/>
+      <c r="C10" s="148"/>
+      <c r="D10" s="148"/>
+      <c r="E10" s="148"/>
+      <c r="F10" s="148"/>
+      <c r="G10" s="148"/>
+      <c r="H10" s="148"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
+      <c r="K10" s="152"/>
+    </row>
+    <row r="11" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A11" s="226" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="227"/>
+      <c r="C11" s="153" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="154"/>
+      <c r="E11" s="153" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="154"/>
+      <c r="G11" s="154"/>
+      <c r="H11" s="153" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="154"/>
+      <c r="J11" s="153" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="155"/>
+    </row>
+    <row r="12" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A12" s="156"/>
+      <c r="B12" s="157"/>
+      <c r="C12" s="158" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="157"/>
+      <c r="E12" s="158" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="158"/>
+      <c r="G12" s="157"/>
+      <c r="H12" s="159" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="157"/>
+      <c r="J12" s="156" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="160"/>
+    </row>
+    <row r="13" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A13" s="161" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="162"/>
+      <c r="C13" s="142"/>
+      <c r="D13" s="162"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="142"/>
+      <c r="G13" s="162"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="162"/>
+      <c r="J13" s="161"/>
+      <c r="K13" s="164"/>
+    </row>
+    <row r="14" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A14" s="161" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="162"/>
+      <c r="C14" s="142"/>
+      <c r="D14" s="162"/>
+      <c r="E14" s="142"/>
+      <c r="F14" s="142"/>
+      <c r="G14" s="162"/>
+      <c r="H14" s="142"/>
+      <c r="I14" s="162"/>
+      <c r="J14" s="161"/>
+      <c r="K14" s="162"/>
+    </row>
+    <row r="15" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A15" s="161" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="162"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="162"/>
+      <c r="E15" s="142"/>
+      <c r="F15" s="142"/>
+      <c r="G15" s="162"/>
+      <c r="H15" s="142"/>
+      <c r="I15" s="162"/>
+      <c r="J15" s="161"/>
+      <c r="K15" s="162"/>
+    </row>
+    <row r="16" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A16" s="165" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="166"/>
+      <c r="C16" s="167"/>
+      <c r="D16" s="166"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="167"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="167"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="166"/>
+    </row>
+    <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="228" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="229"/>
+      <c r="C17" s="229"/>
+      <c r="D17" s="229"/>
+      <c r="E17" s="229"/>
+      <c r="F17" s="229"/>
+      <c r="G17" s="229"/>
+      <c r="H17" s="229"/>
+      <c r="I17" s="229"/>
+      <c r="J17" s="229"/>
+      <c r="K17" s="230"/>
+    </row>
+    <row r="18" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A18" s="231" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="232"/>
+      <c r="C18" s="232"/>
+      <c r="D18" s="233"/>
+      <c r="E18" s="234" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="234"/>
+      <c r="G18" s="234"/>
+      <c r="H18" s="235" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" s="235" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="235" t="s">
+        <v>104</v>
+      </c>
+      <c r="K18" s="234" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A19" s="168" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="168" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="168" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="168" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="168" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="168" t="s">
+        <v>106</v>
+      </c>
+      <c r="G19" s="169" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" s="235"/>
+      <c r="I19" s="235"/>
+      <c r="J19" s="235"/>
+      <c r="K19" s="234"/>
+    </row>
+    <row r="20" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A20" s="168"/>
+      <c r="B20" s="170"/>
+      <c r="C20" s="170"/>
+      <c r="D20" s="170"/>
+      <c r="E20" s="171"/>
+      <c r="F20" s="171"/>
+      <c r="G20" s="171"/>
+      <c r="H20" s="171"/>
+      <c r="I20" s="170"/>
+      <c r="J20" s="172"/>
+      <c r="K20" s="170"/>
+    </row>
+    <row r="21" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A21" s="168"/>
+      <c r="B21" s="170"/>
+      <c r="C21" s="170"/>
+      <c r="D21" s="170"/>
+      <c r="E21" s="171"/>
+      <c r="F21" s="171"/>
+      <c r="G21" s="171"/>
+      <c r="H21" s="171"/>
+      <c r="I21" s="170"/>
+      <c r="J21" s="172"/>
+      <c r="K21" s="173"/>
+    </row>
+    <row r="22" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A22" s="168"/>
+      <c r="B22" s="170"/>
+      <c r="C22" s="170"/>
+      <c r="D22" s="170"/>
+      <c r="E22" s="171"/>
+      <c r="F22" s="171"/>
+      <c r="G22" s="171"/>
+      <c r="H22" s="171"/>
+      <c r="I22" s="170"/>
+      <c r="J22" s="172"/>
+      <c r="K22" s="170"/>
+    </row>
+    <row r="23" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A23" s="168"/>
+      <c r="B23" s="170"/>
+      <c r="C23" s="170"/>
+      <c r="D23" s="170"/>
+      <c r="E23" s="171"/>
+      <c r="F23" s="171"/>
+      <c r="G23" s="171"/>
+      <c r="H23" s="171"/>
+      <c r="I23" s="170"/>
+      <c r="J23" s="172"/>
+      <c r="K23" s="170"/>
+    </row>
+    <row r="24" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A24" s="168"/>
+      <c r="B24" s="170"/>
+      <c r="C24" s="170"/>
+      <c r="D24" s="170"/>
+      <c r="E24" s="171"/>
+      <c r="F24" s="171"/>
+      <c r="G24" s="171"/>
+      <c r="H24" s="171"/>
+      <c r="I24" s="170"/>
+      <c r="J24" s="172"/>
+      <c r="K24" s="170"/>
+    </row>
+    <row r="25" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A25" s="168"/>
+      <c r="B25" s="170"/>
+      <c r="C25" s="170"/>
+      <c r="D25" s="170"/>
+      <c r="E25" s="171"/>
+      <c r="F25" s="171"/>
+      <c r="G25" s="171"/>
+      <c r="H25" s="171"/>
+      <c r="I25" s="170"/>
+      <c r="J25" s="172"/>
+      <c r="K25" s="170"/>
+    </row>
+    <row r="26" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A26" s="168"/>
+      <c r="B26" s="170"/>
+      <c r="C26" s="170"/>
+      <c r="D26" s="170"/>
+      <c r="E26" s="171"/>
+      <c r="F26" s="171"/>
+      <c r="G26" s="171"/>
+      <c r="H26" s="171"/>
+      <c r="I26" s="170"/>
+      <c r="J26" s="172"/>
+      <c r="K26" s="170"/>
+    </row>
+    <row r="27" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A27" s="168"/>
+      <c r="B27" s="170"/>
+      <c r="C27" s="170"/>
+      <c r="D27" s="170"/>
+      <c r="E27" s="171"/>
+      <c r="F27" s="171"/>
+      <c r="G27" s="171"/>
+      <c r="H27" s="171"/>
+      <c r="I27" s="170"/>
+      <c r="J27" s="172"/>
+      <c r="K27" s="170"/>
+    </row>
+    <row r="28" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A28" s="168"/>
+      <c r="B28" s="170"/>
+      <c r="C28" s="170"/>
+      <c r="D28" s="170"/>
+      <c r="E28" s="171"/>
+      <c r="F28" s="171"/>
+      <c r="G28" s="171"/>
+      <c r="H28" s="171"/>
+      <c r="I28" s="170"/>
+      <c r="J28" s="172"/>
+      <c r="K28" s="170"/>
+    </row>
+    <row r="29" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A29" s="168"/>
+      <c r="B29" s="170"/>
+      <c r="C29" s="170"/>
+      <c r="D29" s="170"/>
+      <c r="E29" s="171"/>
+      <c r="F29" s="171"/>
+      <c r="G29" s="171"/>
+      <c r="H29" s="171"/>
+      <c r="I29" s="170"/>
+      <c r="J29" s="172"/>
+      <c r="K29" s="170"/>
+    </row>
+    <row r="30" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A30" s="168"/>
+      <c r="B30" s="170"/>
+      <c r="C30" s="170"/>
+      <c r="D30" s="170"/>
+      <c r="E30" s="171"/>
+      <c r="F30" s="171"/>
+      <c r="G30" s="171"/>
+      <c r="H30" s="171"/>
+      <c r="I30" s="170"/>
+      <c r="J30" s="172"/>
+      <c r="K30" s="170"/>
+    </row>
+    <row r="31" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A31" s="168"/>
+      <c r="B31" s="170"/>
+      <c r="C31" s="170"/>
+      <c r="D31" s="170"/>
+      <c r="E31" s="171"/>
+      <c r="F31" s="171"/>
+      <c r="G31" s="171"/>
+      <c r="H31" s="171"/>
+      <c r="I31" s="170"/>
+      <c r="J31" s="172"/>
+      <c r="K31" s="170"/>
+    </row>
+    <row r="32" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A32" s="171"/>
+      <c r="B32" s="171"/>
+      <c r="C32" s="171"/>
+      <c r="D32" s="171"/>
+      <c r="E32" s="170"/>
+      <c r="F32" s="170"/>
+      <c r="G32" s="170"/>
+      <c r="H32" s="171"/>
+      <c r="I32" s="170"/>
+      <c r="J32" s="170"/>
+      <c r="K32" s="170"/>
+    </row>
+    <row r="33" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A33" s="168"/>
+      <c r="B33" s="170"/>
+      <c r="C33" s="170"/>
+      <c r="D33" s="170"/>
+      <c r="E33" s="171"/>
+      <c r="F33" s="171"/>
+      <c r="G33" s="171"/>
+      <c r="H33" s="171"/>
+      <c r="I33" s="170"/>
+      <c r="J33" s="172"/>
+      <c r="K33" s="170"/>
+    </row>
+    <row r="34" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A34" s="168"/>
+      <c r="B34" s="170"/>
+      <c r="C34" s="170"/>
+      <c r="D34" s="170"/>
+      <c r="E34" s="171"/>
+      <c r="F34" s="171"/>
+      <c r="G34" s="171"/>
+      <c r="H34" s="171"/>
+      <c r="I34" s="170"/>
+      <c r="J34" s="172"/>
+      <c r="K34" s="170"/>
+    </row>
+    <row r="35" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A35" s="168"/>
+      <c r="B35" s="170"/>
+      <c r="C35" s="170"/>
+      <c r="D35" s="170"/>
+      <c r="E35" s="171"/>
+      <c r="F35" s="171"/>
+      <c r="G35" s="171"/>
+      <c r="H35" s="171"/>
+      <c r="I35" s="170"/>
+      <c r="J35" s="172"/>
+      <c r="K35" s="170"/>
+    </row>
+    <row r="36" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A36" s="168"/>
+      <c r="B36" s="170"/>
+      <c r="C36" s="170"/>
+      <c r="D36" s="170"/>
+      <c r="E36" s="171"/>
+      <c r="F36" s="171"/>
+      <c r="G36" s="171"/>
+      <c r="H36" s="171"/>
+      <c r="I36" s="170"/>
+      <c r="J36" s="172"/>
+      <c r="K36" s="170"/>
+    </row>
+    <row r="37" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A37" s="168"/>
+      <c r="B37" s="170"/>
+      <c r="C37" s="170"/>
+      <c r="D37" s="170"/>
+      <c r="E37" s="171"/>
+      <c r="F37" s="171"/>
+      <c r="G37" s="171"/>
+      <c r="H37" s="171"/>
+      <c r="I37" s="170"/>
+      <c r="J37" s="172"/>
+      <c r="K37" s="170"/>
+    </row>
+    <row r="38" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A38" s="168"/>
+      <c r="B38" s="170"/>
+      <c r="C38" s="170"/>
+      <c r="D38" s="170"/>
+      <c r="E38" s="171"/>
+      <c r="F38" s="171"/>
+      <c r="G38" s="171"/>
+      <c r="H38" s="171"/>
+      <c r="I38" s="170"/>
+      <c r="J38" s="172"/>
+      <c r="K38" s="170"/>
+    </row>
+    <row r="39" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A39" s="168"/>
+      <c r="B39" s="170"/>
+      <c r="C39" s="170"/>
+      <c r="D39" s="170"/>
+      <c r="E39" s="171"/>
+      <c r="F39" s="171"/>
+      <c r="G39" s="171"/>
+      <c r="H39" s="171"/>
+      <c r="I39" s="170"/>
+      <c r="J39" s="172"/>
+      <c r="K39" s="170"/>
+    </row>
+    <row r="40" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A40" s="168"/>
+      <c r="B40" s="170"/>
+      <c r="C40" s="170"/>
+      <c r="D40" s="170"/>
+      <c r="E40" s="171"/>
+      <c r="F40" s="171"/>
+      <c r="G40" s="171"/>
+      <c r="H40" s="171"/>
+      <c r="I40" s="170"/>
+      <c r="J40" s="172"/>
+      <c r="K40" s="170"/>
+    </row>
+    <row r="41" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A41" s="168"/>
+      <c r="B41" s="170"/>
+      <c r="C41" s="170"/>
+      <c r="D41" s="170"/>
+      <c r="E41" s="171"/>
+      <c r="F41" s="171"/>
+      <c r="G41" s="171"/>
+      <c r="H41" s="171"/>
+      <c r="I41" s="170"/>
+      <c r="J41" s="172"/>
+      <c r="K41" s="170"/>
+    </row>
+    <row r="42" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A42" s="168"/>
+      <c r="B42" s="170"/>
+      <c r="C42" s="170"/>
+      <c r="D42" s="170"/>
+      <c r="E42" s="171"/>
+      <c r="F42" s="171"/>
+      <c r="G42" s="171"/>
+      <c r="H42" s="171"/>
+      <c r="I42" s="170"/>
+      <c r="J42" s="172"/>
+      <c r="K42" s="170"/>
+    </row>
+    <row r="43" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A43" s="168"/>
+      <c r="B43" s="170"/>
+      <c r="C43" s="170"/>
+      <c r="D43" s="170"/>
+      <c r="E43" s="171"/>
+      <c r="F43" s="171"/>
+      <c r="G43" s="171"/>
+      <c r="H43" s="171"/>
+      <c r="I43" s="170"/>
+      <c r="J43" s="172"/>
+      <c r="K43" s="170"/>
+    </row>
+    <row r="44" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A44" s="168"/>
+      <c r="B44" s="170"/>
+      <c r="C44" s="170"/>
+      <c r="D44" s="170"/>
+      <c r="E44" s="171"/>
+      <c r="F44" s="171"/>
+      <c r="G44" s="171"/>
+      <c r="H44" s="171"/>
+      <c r="I44" s="170"/>
+      <c r="J44" s="172"/>
+      <c r="K44" s="170"/>
+    </row>
+    <row r="45" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A45" s="168"/>
+      <c r="B45" s="170"/>
+      <c r="C45" s="170"/>
+      <c r="D45" s="170"/>
+      <c r="E45" s="171"/>
+      <c r="F45" s="171"/>
+      <c r="G45" s="171"/>
+      <c r="H45" s="171"/>
+      <c r="I45" s="170"/>
+      <c r="J45" s="172"/>
+      <c r="K45" s="170"/>
+    </row>
+    <row r="46" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A46" s="168"/>
+      <c r="B46" s="170"/>
+      <c r="C46" s="170"/>
+      <c r="D46" s="170"/>
+      <c r="E46" s="171"/>
+      <c r="F46" s="171"/>
+      <c r="G46" s="171"/>
+      <c r="H46" s="171"/>
+      <c r="I46" s="170"/>
+      <c r="J46" s="172"/>
+      <c r="K46" s="170"/>
+    </row>
+    <row r="47" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A47" s="168"/>
+      <c r="B47" s="170"/>
+      <c r="C47" s="170"/>
+      <c r="D47" s="170"/>
+      <c r="E47" s="171"/>
+      <c r="F47" s="171"/>
+      <c r="G47" s="171"/>
+      <c r="H47" s="171"/>
+      <c r="I47" s="170"/>
+      <c r="J47" s="172"/>
+      <c r="K47" s="170"/>
+    </row>
+    <row r="48" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A48" s="168"/>
+      <c r="B48" s="170"/>
+      <c r="C48" s="170"/>
+      <c r="D48" s="170"/>
+      <c r="E48" s="171"/>
+      <c r="F48" s="171"/>
+      <c r="G48" s="171"/>
+      <c r="H48" s="171"/>
+      <c r="I48" s="170"/>
+      <c r="J48" s="172"/>
+      <c r="K48" s="170"/>
+    </row>
+    <row r="49" spans="1:11" ht="12" x14ac:dyDescent="0.25">
+      <c r="A49" s="168"/>
+      <c r="B49" s="170"/>
+      <c r="C49" s="170"/>
+      <c r="D49" s="170"/>
+      <c r="E49" s="171"/>
+      <c r="F49" s="171"/>
+      <c r="G49" s="171"/>
+      <c r="H49" s="171"/>
+      <c r="I49" s="170"/>
+      <c r="J49" s="172"/>
+      <c r="K49" s="170"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="174"/>
+      <c r="B50" s="175"/>
+      <c r="C50" s="175"/>
+      <c r="D50" s="175"/>
+      <c r="E50" s="175"/>
+      <c r="F50" s="175"/>
+      <c r="G50" s="175"/>
+      <c r="H50" s="175"/>
+      <c r="I50" s="175"/>
+      <c r="J50" s="175"/>
+      <c r="K50" s="175"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="174"/>
+      <c r="B51" s="175"/>
+      <c r="C51" s="175"/>
+      <c r="D51" s="175"/>
+      <c r="E51" s="175"/>
+      <c r="F51" s="175"/>
+      <c r="G51" s="175"/>
+      <c r="H51" s="175"/>
+      <c r="I51" s="175"/>
+      <c r="J51" s="175"/>
+      <c r="K51" s="175"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="174"/>
+      <c r="B52" s="175"/>
+      <c r="C52" s="175"/>
+      <c r="D52" s="175"/>
+      <c r="E52" s="175"/>
+      <c r="F52" s="175"/>
+      <c r="G52" s="175"/>
+      <c r="H52" s="175"/>
+      <c r="I52" s="175"/>
+      <c r="J52" s="175"/>
+      <c r="K52" s="175"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="174"/>
+      <c r="B53" s="175"/>
+      <c r="C53" s="175"/>
+      <c r="D53" s="175"/>
+      <c r="E53" s="175"/>
+      <c r="F53" s="175"/>
+      <c r="G53" s="175"/>
+      <c r="H53" s="175"/>
+      <c r="I53" s="175"/>
+      <c r="J53" s="175"/>
+      <c r="K53" s="175"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="174"/>
+      <c r="B54" s="175"/>
+      <c r="C54" s="175"/>
+      <c r="D54" s="175"/>
+      <c r="E54" s="175"/>
+      <c r="F54" s="175"/>
+      <c r="G54" s="175"/>
+      <c r="H54" s="175"/>
+      <c r="I54" s="175"/>
+      <c r="J54" s="175"/>
+      <c r="K54" s="175"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="174"/>
+      <c r="B55" s="175"/>
+      <c r="C55" s="175"/>
+      <c r="D55" s="175"/>
+      <c r="E55" s="175"/>
+      <c r="F55" s="175"/>
+      <c r="G55" s="175"/>
+      <c r="H55" s="175"/>
+      <c r="I55" s="175"/>
+      <c r="J55" s="175"/>
+      <c r="K55" s="175"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="174"/>
+      <c r="B56" s="175"/>
+      <c r="C56" s="175"/>
+      <c r="D56" s="175"/>
+      <c r="E56" s="175"/>
+      <c r="F56" s="175"/>
+      <c r="G56" s="175"/>
+      <c r="H56" s="175"/>
+      <c r="I56" s="175"/>
+      <c r="J56" s="175"/>
+      <c r="K56" s="175"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="174"/>
+      <c r="B57" s="175"/>
+      <c r="C57" s="175"/>
+      <c r="D57" s="175"/>
+      <c r="E57" s="175"/>
+      <c r="F57" s="175"/>
+      <c r="G57" s="175"/>
+      <c r="H57" s="175"/>
+      <c r="I57" s="175"/>
+      <c r="J57" s="175"/>
+      <c r="K57" s="175"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="174"/>
+      <c r="B58" s="175"/>
+      <c r="C58" s="175"/>
+      <c r="D58" s="175"/>
+      <c r="E58" s="175"/>
+      <c r="F58" s="175"/>
+      <c r="G58" s="175"/>
+      <c r="H58" s="175"/>
+      <c r="I58" s="175"/>
+      <c r="J58" s="175"/>
+      <c r="K58" s="175"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="174"/>
+      <c r="B59" s="175"/>
+      <c r="C59" s="175"/>
+      <c r="D59" s="175"/>
+      <c r="E59" s="175"/>
+      <c r="F59" s="175"/>
+      <c r="G59" s="175"/>
+      <c r="H59" s="175"/>
+      <c r="I59" s="175"/>
+      <c r="J59" s="175"/>
+      <c r="K59" s="175"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="174"/>
+      <c r="B60" s="175"/>
+      <c r="C60" s="175"/>
+      <c r="D60" s="175"/>
+      <c r="E60" s="175"/>
+      <c r="F60" s="175"/>
+      <c r="G60" s="175"/>
+      <c r="H60" s="175"/>
+      <c r="I60" s="175"/>
+      <c r="J60" s="175"/>
+      <c r="K60" s="175"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="174"/>
+      <c r="B61" s="175"/>
+      <c r="C61" s="175"/>
+      <c r="D61" s="175"/>
+      <c r="E61" s="175"/>
+      <c r="F61" s="175"/>
+      <c r="G61" s="175"/>
+      <c r="H61" s="175"/>
+      <c r="I61" s="175"/>
+      <c r="J61" s="175"/>
+      <c r="K61" s="175"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="174"/>
+      <c r="B62" s="175"/>
+      <c r="C62" s="175"/>
+      <c r="D62" s="175"/>
+      <c r="E62" s="175"/>
+      <c r="F62" s="175"/>
+      <c r="G62" s="175"/>
+      <c r="H62" s="175"/>
+      <c r="I62" s="175"/>
+      <c r="J62" s="175"/>
+      <c r="K62" s="175"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="174"/>
+      <c r="B63" s="175"/>
+      <c r="C63" s="175"/>
+      <c r="D63" s="175"/>
+      <c r="E63" s="175"/>
+      <c r="F63" s="175"/>
+      <c r="G63" s="175"/>
+      <c r="H63" s="175"/>
+      <c r="I63" s="175"/>
+      <c r="J63" s="175"/>
+      <c r="K63" s="175"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="174"/>
+      <c r="B64" s="175"/>
+      <c r="C64" s="175"/>
+      <c r="D64" s="175"/>
+      <c r="E64" s="175"/>
+      <c r="F64" s="175"/>
+      <c r="G64" s="175"/>
+      <c r="H64" s="175"/>
+      <c r="I64" s="175"/>
+      <c r="J64" s="175"/>
+      <c r="K64" s="175"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="174"/>
+      <c r="B65" s="175"/>
+      <c r="C65" s="175"/>
+      <c r="D65" s="175"/>
+      <c r="E65" s="175"/>
+      <c r="F65" s="175"/>
+      <c r="G65" s="175"/>
+      <c r="H65" s="175"/>
+      <c r="I65" s="175"/>
+      <c r="J65" s="175"/>
+      <c r="K65" s="175"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="174"/>
+      <c r="B66" s="175"/>
+      <c r="C66" s="175"/>
+      <c r="D66" s="175"/>
+      <c r="E66" s="175"/>
+      <c r="F66" s="175"/>
+      <c r="G66" s="175"/>
+      <c r="H66" s="175"/>
+      <c r="I66" s="175"/>
+      <c r="J66" s="175"/>
+      <c r="K66" s="175"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="174"/>
+      <c r="B67" s="175"/>
+      <c r="C67" s="175"/>
+      <c r="D67" s="175"/>
+      <c r="E67" s="175"/>
+      <c r="F67" s="175"/>
+      <c r="G67" s="175"/>
+      <c r="H67" s="175"/>
+      <c r="I67" s="175"/>
+      <c r="J67" s="175"/>
+      <c r="K67" s="175"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="174"/>
+      <c r="B68" s="175"/>
+      <c r="C68" s="175"/>
+      <c r="D68" s="175"/>
+      <c r="E68" s="175"/>
+      <c r="F68" s="175"/>
+      <c r="G68" s="175"/>
+      <c r="H68" s="175"/>
+      <c r="I68" s="175"/>
+      <c r="J68" s="175"/>
+      <c r="K68" s="175"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="174"/>
+      <c r="B69" s="175"/>
+      <c r="C69" s="175"/>
+      <c r="D69" s="175"/>
+      <c r="E69" s="175"/>
+      <c r="F69" s="175"/>
+      <c r="G69" s="175"/>
+      <c r="H69" s="175"/>
+      <c r="I69" s="175"/>
+      <c r="J69" s="175"/>
+      <c r="K69" s="175"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="174"/>
+      <c r="B70" s="175"/>
+      <c r="C70" s="175"/>
+      <c r="D70" s="175"/>
+      <c r="E70" s="175"/>
+      <c r="F70" s="175"/>
+      <c r="G70" s="175"/>
+      <c r="H70" s="175"/>
+      <c r="I70" s="175"/>
+      <c r="J70" s="175"/>
+      <c r="K70" s="175"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="174"/>
+      <c r="B71" s="175"/>
+      <c r="C71" s="175"/>
+      <c r="D71" s="175"/>
+      <c r="E71" s="175"/>
+      <c r="F71" s="175"/>
+      <c r="G71" s="175"/>
+      <c r="H71" s="175"/>
+      <c r="I71" s="175"/>
+      <c r="J71" s="175"/>
+      <c r="K71" s="175"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="174"/>
+      <c r="B72" s="175"/>
+      <c r="C72" s="175"/>
+      <c r="D72" s="175"/>
+      <c r="E72" s="175"/>
+      <c r="F72" s="175"/>
+      <c r="G72" s="175"/>
+      <c r="H72" s="175"/>
+      <c r="I72" s="175"/>
+      <c r="J72" s="175"/>
+      <c r="K72" s="175"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="174"/>
+      <c r="B73" s="175"/>
+      <c r="C73" s="175"/>
+      <c r="D73" s="175"/>
+      <c r="E73" s="175"/>
+      <c r="F73" s="175"/>
+      <c r="G73" s="175"/>
+      <c r="H73" s="175"/>
+      <c r="I73" s="175"/>
+      <c r="J73" s="175"/>
+      <c r="K73" s="175"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="174"/>
+      <c r="B74" s="175"/>
+      <c r="C74" s="175"/>
+      <c r="D74" s="175"/>
+      <c r="E74" s="175"/>
+      <c r="F74" s="175"/>
+      <c r="G74" s="175"/>
+      <c r="H74" s="175"/>
+      <c r="I74" s="175"/>
+      <c r="J74" s="175"/>
+      <c r="K74" s="175"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="174"/>
+      <c r="B75" s="175"/>
+      <c r="C75" s="175"/>
+      <c r="D75" s="175"/>
+      <c r="E75" s="175"/>
+      <c r="F75" s="175"/>
+      <c r="G75" s="175"/>
+      <c r="H75" s="175"/>
+      <c r="I75" s="175"/>
+      <c r="J75" s="175"/>
+      <c r="K75" s="175"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="174"/>
+      <c r="B76" s="175"/>
+      <c r="C76" s="175"/>
+      <c r="D76" s="175"/>
+      <c r="E76" s="175"/>
+      <c r="F76" s="175"/>
+      <c r="G76" s="175"/>
+      <c r="H76" s="175"/>
+      <c r="I76" s="175"/>
+      <c r="J76" s="175"/>
+      <c r="K76" s="175"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="174"/>
+      <c r="B77" s="175"/>
+      <c r="C77" s="175"/>
+      <c r="D77" s="175"/>
+      <c r="E77" s="175"/>
+      <c r="F77" s="175"/>
+      <c r="G77" s="175"/>
+      <c r="H77" s="175"/>
+      <c r="I77" s="175"/>
+      <c r="J77" s="175"/>
+      <c r="K77" s="175"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="174"/>
+      <c r="B78" s="175"/>
+      <c r="C78" s="175"/>
+      <c r="D78" s="175"/>
+      <c r="E78" s="175"/>
+      <c r="F78" s="175"/>
+      <c r="G78" s="175"/>
+      <c r="H78" s="175"/>
+      <c r="I78" s="175"/>
+      <c r="J78" s="175"/>
+      <c r="K78" s="175"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="174"/>
+      <c r="B79" s="175"/>
+      <c r="C79" s="175"/>
+      <c r="D79" s="175"/>
+      <c r="E79" s="175"/>
+      <c r="F79" s="175"/>
+      <c r="G79" s="175"/>
+      <c r="H79" s="175"/>
+      <c r="I79" s="175"/>
+      <c r="J79" s="175"/>
+      <c r="K79" s="175"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="174"/>
+      <c r="B80" s="175"/>
+      <c r="C80" s="175"/>
+      <c r="D80" s="175"/>
+      <c r="E80" s="175"/>
+      <c r="F80" s="175"/>
+      <c r="G80" s="175"/>
+      <c r="H80" s="175"/>
+      <c r="I80" s="175"/>
+      <c r="J80" s="175"/>
+      <c r="K80" s="175"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="174"/>
+      <c r="B81" s="175"/>
+      <c r="C81" s="175"/>
+      <c r="D81" s="175"/>
+      <c r="E81" s="175"/>
+      <c r="F81" s="175"/>
+      <c r="G81" s="175"/>
+      <c r="H81" s="175"/>
+      <c r="I81" s="175"/>
+      <c r="J81" s="175"/>
+      <c r="K81" s="175"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="174"/>
+      <c r="B82" s="175"/>
+      <c r="C82" s="175"/>
+      <c r="D82" s="175"/>
+      <c r="E82" s="175"/>
+      <c r="F82" s="175"/>
+      <c r="G82" s="175"/>
+      <c r="H82" s="175"/>
+      <c r="I82" s="175"/>
+      <c r="J82" s="175"/>
+      <c r="K82" s="175"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="174"/>
+      <c r="B83" s="175"/>
+      <c r="C83" s="175"/>
+      <c r="D83" s="175"/>
+      <c r="E83" s="175"/>
+      <c r="F83" s="175"/>
+      <c r="G83" s="175"/>
+      <c r="H83" s="175"/>
+      <c r="I83" s="175"/>
+      <c r="J83" s="175"/>
+      <c r="K83" s="175"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="174"/>
+      <c r="B84" s="175"/>
+      <c r="C84" s="175"/>
+      <c r="D84" s="175"/>
+      <c r="E84" s="175"/>
+      <c r="F84" s="175"/>
+      <c r="G84" s="175"/>
+      <c r="H84" s="175"/>
+      <c r="I84" s="175"/>
+      <c r="J84" s="175"/>
+      <c r="K84" s="175"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="174"/>
+      <c r="B85" s="175"/>
+      <c r="C85" s="175"/>
+      <c r="D85" s="175"/>
+      <c r="E85" s="175"/>
+      <c r="F85" s="175"/>
+      <c r="G85" s="175"/>
+      <c r="H85" s="175"/>
+      <c r="I85" s="175"/>
+      <c r="J85" s="175"/>
+      <c r="K85" s="175"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="174"/>
+      <c r="B86" s="175"/>
+      <c r="C86" s="175"/>
+      <c r="D86" s="175"/>
+      <c r="E86" s="175"/>
+      <c r="F86" s="175"/>
+      <c r="G86" s="175"/>
+      <c r="H86" s="175"/>
+      <c r="I86" s="175"/>
+      <c r="J86" s="175"/>
+      <c r="K86" s="175"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="174"/>
+      <c r="B87" s="175"/>
+      <c r="C87" s="175"/>
+      <c r="D87" s="175"/>
+      <c r="E87" s="175"/>
+      <c r="F87" s="175"/>
+      <c r="G87" s="175"/>
+      <c r="H87" s="175"/>
+      <c r="I87" s="175"/>
+      <c r="J87" s="175"/>
+      <c r="K87" s="175"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="174"/>
+      <c r="B88" s="175"/>
+      <c r="C88" s="175"/>
+      <c r="D88" s="175"/>
+      <c r="E88" s="175"/>
+      <c r="F88" s="175"/>
+      <c r="G88" s="175"/>
+      <c r="H88" s="175"/>
+      <c r="I88" s="175"/>
+      <c r="J88" s="175"/>
+      <c r="K88" s="175"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="174"/>
+      <c r="B89" s="175"/>
+      <c r="C89" s="175"/>
+      <c r="D89" s="175"/>
+      <c r="E89" s="175"/>
+      <c r="F89" s="175"/>
+      <c r="G89" s="175"/>
+      <c r="H89" s="175"/>
+      <c r="I89" s="175"/>
+      <c r="J89" s="175"/>
+      <c r="K89" s="175"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="174"/>
+      <c r="B90" s="175"/>
+      <c r="C90" s="175"/>
+      <c r="D90" s="175"/>
+      <c r="E90" s="175"/>
+      <c r="F90" s="175"/>
+      <c r="G90" s="175"/>
+      <c r="H90" s="175"/>
+      <c r="I90" s="175"/>
+      <c r="J90" s="175"/>
+      <c r="K90" s="175"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="174"/>
+      <c r="B91" s="175"/>
+      <c r="C91" s="175"/>
+      <c r="D91" s="175"/>
+      <c r="E91" s="175"/>
+      <c r="F91" s="175"/>
+      <c r="G91" s="175"/>
+      <c r="H91" s="175"/>
+      <c r="I91" s="175"/>
+      <c r="J91" s="175"/>
+      <c r="K91" s="175"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="174"/>
+      <c r="B92" s="175"/>
+      <c r="C92" s="175"/>
+      <c r="D92" s="175"/>
+      <c r="E92" s="175"/>
+      <c r="F92" s="175"/>
+      <c r="G92" s="175"/>
+      <c r="H92" s="175"/>
+      <c r="I92" s="175"/>
+      <c r="J92" s="175"/>
+      <c r="K92" s="175"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="174"/>
+      <c r="B93" s="175"/>
+      <c r="C93" s="175"/>
+      <c r="D93" s="175"/>
+      <c r="E93" s="175"/>
+      <c r="F93" s="175"/>
+      <c r="G93" s="175"/>
+      <c r="H93" s="175"/>
+      <c r="I93" s="175"/>
+      <c r="J93" s="175"/>
+      <c r="K93" s="175"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="174"/>
+      <c r="B94" s="175"/>
+      <c r="C94" s="175"/>
+      <c r="D94" s="175"/>
+      <c r="E94" s="175"/>
+      <c r="F94" s="175"/>
+      <c r="G94" s="175"/>
+      <c r="H94" s="175"/>
+      <c r="I94" s="175"/>
+      <c r="J94" s="175"/>
+      <c r="K94" s="175"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="174"/>
+      <c r="B95" s="175"/>
+      <c r="C95" s="175"/>
+      <c r="D95" s="175"/>
+      <c r="E95" s="175"/>
+      <c r="F95" s="175"/>
+      <c r="G95" s="175"/>
+      <c r="H95" s="175"/>
+      <c r="I95" s="175"/>
+      <c r="J95" s="175"/>
+      <c r="K95" s="175"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="174"/>
+      <c r="B96" s="175"/>
+      <c r="C96" s="175"/>
+      <c r="D96" s="175"/>
+      <c r="E96" s="175"/>
+      <c r="F96" s="175"/>
+      <c r="G96" s="175"/>
+      <c r="H96" s="175"/>
+      <c r="I96" s="175"/>
+      <c r="J96" s="175"/>
+      <c r="K96" s="175"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+  </mergeCells>
+  <pageMargins left="0.21" right="0.17" top="0.75" bottom="0.52" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="28" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed final fuel report system
</commit_message>
<xml_diff>
--- a/public/templates/template_file.xlsx
+++ b/public/templates/template_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Inventory 2081-82 developmentfolder\inventory-backend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFC0D70-9010-47BE-8395-21F0919C7B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC412A9-5FF5-46D9-AF77-882ABD0A869D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Request Template" sheetId="21" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="RRLP Template" sheetId="23" r:id="rId3"/>
     <sheet name="Stock Card Template" sheetId="24" r:id="rId4"/>
     <sheet name="Diesel Weekly Template" sheetId="25" r:id="rId5"/>
+    <sheet name="Oil Weekly Template" sheetId="28" r:id="rId6"/>
+    <sheet name="Petrol Weekly Template" sheetId="26" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="168">
   <si>
     <t>U/M</t>
   </si>
@@ -444,91 +445,109 @@
     <t>Remaining Budget on Surface Fuel (B-10-97)</t>
   </si>
   <si>
+    <t>207T</t>
+  </si>
+  <si>
+    <t>344T14</t>
+  </si>
+  <si>
+    <t>345T15</t>
+  </si>
+  <si>
+    <t>346T42</t>
+  </si>
+  <si>
+    <t>444T44</t>
+  </si>
+  <si>
+    <t>634T47</t>
+  </si>
+  <si>
+    <t>1512T</t>
+  </si>
+  <si>
+    <t>1709T10</t>
+  </si>
+  <si>
+    <t>New GSE Thai</t>
+  </si>
+  <si>
+    <t>Karcher</t>
+  </si>
+  <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>GS &amp; PMD</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Automatic Cut-off Fuel dispensing nozzle</t>
+  </si>
+  <si>
+    <t>No IAI found</t>
+  </si>
+  <si>
+    <t>As provided by GSE Operation Section</t>
+  </si>
+  <si>
+    <t>Excluding the diesel payment used in GE 1237 and petrol as payment done from GS&amp;PMD</t>
+  </si>
+  <si>
+    <t>GSE Stores</t>
+  </si>
+  <si>
+    <t>Daily Fuel Entry Form (Diesel)</t>
+  </si>
+  <si>
+    <t>Weekly Fuel Consumtion Report (Petrol)</t>
+  </si>
+  <si>
+    <t>Hrm</t>
+  </si>
+  <si>
+    <t>Total Fuel per week</t>
+  </si>
+  <si>
+    <t>Total Fuel consumption of Day</t>
+  </si>
+  <si>
     <t>Prepared By</t>
   </si>
   <si>
-    <t>Checked By:</t>
-  </si>
-  <si>
-    <t>Reviewed/Submitted By</t>
-  </si>
-  <si>
-    <t>Anita KC</t>
-  </si>
-  <si>
-    <t>Saman Tripathee</t>
-  </si>
-  <si>
-    <t>Deependra Bhatta</t>
-  </si>
-  <si>
-    <t>Helper, Inventory Section</t>
-  </si>
-  <si>
-    <t>Technical Expert, Inventory Section</t>
-  </si>
-  <si>
-    <t>In-Charge, Inventroy Section</t>
-  </si>
-  <si>
-    <t>207T</t>
-  </si>
-  <si>
-    <t>344T14</t>
-  </si>
-  <si>
-    <t>345T15</t>
-  </si>
-  <si>
-    <t>346T42</t>
-  </si>
-  <si>
-    <t>444T44</t>
-  </si>
-  <si>
-    <t>634T47</t>
-  </si>
-  <si>
-    <t>1512T</t>
-  </si>
-  <si>
-    <t>1709T10</t>
-  </si>
-  <si>
-    <t>New GSE Thai</t>
-  </si>
-  <si>
-    <t>Karcher</t>
-  </si>
-  <si>
-    <t>Cleaning</t>
-  </si>
-  <si>
-    <t>GS &amp; PMD</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Automatic Cut-off Fuel dispensing nozzle</t>
-  </si>
-  <si>
-    <t>No IAI found</t>
-  </si>
-  <si>
-    <t>As provided by GSE Operation Section</t>
-  </si>
-  <si>
-    <t>Excluding the diesel payment used in GE 1237 and petrol as payment done from GS&amp;PMD</t>
-  </si>
-  <si>
-    <t>GSE Stores</t>
-  </si>
-  <si>
-    <t>Daily Fuel Entry Form (Diesel)</t>
-  </si>
-  <si>
-    <t>Reason for the change in Total Cost: Decrease in Diesel consumtion even decrease in rate of diesel by NPR 1/Lt effective from 2082/02/22.</t>
+    <t>Checked By</t>
+  </si>
+  <si>
+    <t>Reviewed/submitted By</t>
+  </si>
+  <si>
+    <t>From:</t>
+  </si>
+  <si>
+    <t>GSE Inventory</t>
+  </si>
+  <si>
+    <t>To:</t>
+  </si>
+  <si>
+    <t>GSE R&amp;D Section</t>
+  </si>
+  <si>
+    <t>Weekly Statistics of Activities</t>
+  </si>
+  <si>
+    <t>Week No.</t>
+  </si>
+  <si>
+    <t>Oil Specifications</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Consumed Quantity</t>
   </si>
 </sst>
 </file>
@@ -540,7 +559,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -756,6 +775,25 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -960,7 +998,7 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="282">
+  <cellXfs count="312">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1504,6 +1542,34 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1549,36 +1615,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="40"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="40"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="40"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="40"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1602,6 +1654,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="38"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="45"/>
     </xf>
@@ -1638,12 +1710,6 @@
     <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1673,9 +1739,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1693,19 +1756,32 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1715,25 +1791,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2078,7 +2192,7 @@
             <c:numRef>
               <c:f>('[1]48'!$F$159:$F$160,'[1]48'!$F$162:$F$166)</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>5514</c:v>
@@ -2095,10 +2209,10 @@
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>349</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>349</c:v>
                 </c:pt>
               </c:numCache>
@@ -2636,7 +2750,7 @@
             <c:numRef>
               <c:f>'[1]48'!$F$170:$F$171</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>785497</c:v>
@@ -3209,7 +3323,7 @@
             <c:numRef>
               <c:f>('[1]48'!$F$159:$F$160,'[1]48'!$F$162:$F$166)</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>5514</c:v>
@@ -3226,10 +3340,10 @@
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>349</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>349</c:v>
                 </c:pt>
               </c:numCache>
@@ -3767,7 +3881,7 @@
             <c:numRef>
               <c:f>'[1]48'!$F$170:$F$171</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>785497</c:v>
@@ -4096,13 +4210,7 @@
             <c:strRef>
               <c:f>('Diesel Weekly Template'!$B$159:$B$160,'Diesel Weekly Template'!$B$162:$B$166)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Previous Week (-1) Consumption (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Previous Week () Consumption (in Ltrs)</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
                 <c:pt idx="2">
                   <c:v>Estimated Spillage while Refuelling (in Ltrs)</c:v>
                 </c:pt>
@@ -4111,12 +4219,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fuel Wasted (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total number of flights handled in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Total number of flights handled in Week ()</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4153,13 +4255,7 @@
             <c:strRef>
               <c:f>('Diesel Weekly Template'!$B$159:$B$160,'Diesel Weekly Template'!$B$162:$B$166)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Previous Week (-1) Consumption (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Previous Week () Consumption (in Ltrs)</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
                 <c:pt idx="2">
                   <c:v>Estimated Spillage while Refuelling (in Ltrs)</c:v>
                 </c:pt>
@@ -4168,12 +4264,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fuel Wasted (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total number of flights handled in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Total number of flights handled in Week ()</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4210,13 +4300,7 @@
             <c:strRef>
               <c:f>('Diesel Weekly Template'!$B$159:$B$160,'Diesel Weekly Template'!$B$162:$B$166)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Previous Week (-1) Consumption (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Previous Week () Consumption (in Ltrs)</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
                 <c:pt idx="2">
                   <c:v>Estimated Spillage while Refuelling (in Ltrs)</c:v>
                 </c:pt>
@@ -4225,12 +4309,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fuel Wasted (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total number of flights handled in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Total number of flights handled in Week ()</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4311,13 +4389,7 @@
             <c:strRef>
               <c:f>('Diesel Weekly Template'!$B$159:$B$160,'Diesel Weekly Template'!$B$162:$B$166)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Previous Week (-1) Consumption (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Previous Week () Consumption (in Ltrs)</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
                 <c:pt idx="2">
                   <c:v>Estimated Spillage while Refuelling (in Ltrs)</c:v>
                 </c:pt>
@@ -4326,12 +4398,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fuel Wasted (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total number of flights handled in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Total number of flights handled in Week ()</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4342,12 +4408,6 @@
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4389,13 +4449,7 @@
             <c:strRef>
               <c:f>('Diesel Weekly Template'!$B$159:$B$160,'Diesel Weekly Template'!$B$162:$B$166)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Previous Week (-1) Consumption (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Previous Week () Consumption (in Ltrs)</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
                 <c:pt idx="2">
                   <c:v>Estimated Spillage while Refuelling (in Ltrs)</c:v>
                 </c:pt>
@@ -4404,12 +4458,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fuel Wasted (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total number of flights handled in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Total number of flights handled in Week ()</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4446,13 +4494,7 @@
             <c:strRef>
               <c:f>('Diesel Weekly Template'!$B$159:$B$160,'Diesel Weekly Template'!$B$162:$B$166)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Previous Week (-1) Consumption (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Previous Week () Consumption (in Ltrs)</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
                 <c:pt idx="2">
                   <c:v>Estimated Spillage while Refuelling (in Ltrs)</c:v>
                 </c:pt>
@@ -4461,12 +4503,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fuel Wasted (in Ltrs)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Total number of flights handled in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Total number of flights handled in Week ()</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4711,18 +4747,13 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Diesel Weekly Template'!$B$170:$B$171</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Total cost of diesel issued in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total cost of diesel issued in Week ()</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -4753,18 +4784,13 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Diesel Weekly Template'!$B$170:$B$171</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Total cost of diesel issued in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total cost of diesel issued in Week ()</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -4795,18 +4821,13 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Diesel Weekly Template'!$B$170:$B$171</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Total cost of diesel issued in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total cost of diesel issued in Week ()</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -4881,18 +4902,13 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Diesel Weekly Template'!$B$170:$B$171</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Total cost of diesel issued in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total cost of diesel issued in Week ()</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -4900,12 +4916,6 @@
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4929,18 +4939,13 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Diesel Weekly Template'!$B$170:$B$171</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Total cost of diesel issued in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total cost of diesel issued in Week ()</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -4971,18 +4976,13 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'Diesel Weekly Template'!$B$170:$B$171</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Total cost of diesel issued in Week (-1)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total cost of diesel issued in Week ()</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -5515,6 +5515,51 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1362075" cy="485775"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr="Picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D01538A-911B-4879-BBB6-EEEDA7E4B078}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1362075" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -5620,76 +5665,67 @@
       <sheetData sheetId="45"/>
       <sheetData sheetId="46">
         <row r="159">
-          <cell r="B159" t="str">
-            <v>Previous Week (46) Consumption (in Ltrs)</v>
-          </cell>
-          <cell r="F159">
-            <v>6664</v>
-          </cell>
+          <cell r="C159"/>
+          <cell r="D159"/>
+          <cell r="E159"/>
+          <cell r="G159"/>
+          <cell r="H159"/>
         </row>
         <row r="160">
-          <cell r="B160" t="str">
-            <v>Previous Week (47) Consumption (in Ltrs)</v>
-          </cell>
-          <cell r="F160">
-            <v>5514</v>
-          </cell>
+          <cell r="C160"/>
+          <cell r="D160"/>
+          <cell r="E160"/>
+          <cell r="G160"/>
+          <cell r="H160"/>
         </row>
         <row r="162">
-          <cell r="B162" t="str">
-            <v>Estimated Spillage while Refuelling (in Ltrs)</v>
-          </cell>
-          <cell r="F162" t="str">
-            <v>-</v>
-          </cell>
+          <cell r="C162"/>
+          <cell r="D162"/>
+          <cell r="E162"/>
+          <cell r="G162"/>
+          <cell r="H162"/>
         </row>
         <row r="163">
-          <cell r="B163" t="str">
-            <v>Estmated Leakages in GSE (in Ltrs)</v>
-          </cell>
-          <cell r="F163" t="str">
-            <v>-</v>
-          </cell>
+          <cell r="C163"/>
+          <cell r="D163"/>
+          <cell r="E163"/>
+          <cell r="G163"/>
+          <cell r="H163"/>
         </row>
         <row r="164">
-          <cell r="B164" t="str">
-            <v>Fuel Wasted (in Ltrs)</v>
-          </cell>
-          <cell r="F164" t="str">
-            <v>-</v>
-          </cell>
+          <cell r="C164"/>
+          <cell r="D164"/>
+          <cell r="E164"/>
+          <cell r="G164"/>
+          <cell r="H164"/>
         </row>
         <row r="165">
-          <cell r="B165" t="str">
-            <v>Total number of flights handled in Week (46)</v>
-          </cell>
-          <cell r="F165">
-            <v>349</v>
-          </cell>
+          <cell r="C165"/>
+          <cell r="D165"/>
+          <cell r="E165"/>
+          <cell r="G165"/>
+          <cell r="H165"/>
         </row>
         <row r="166">
-          <cell r="B166" t="str">
-            <v>Total number of flights handled in Week (47)</v>
-          </cell>
-          <cell r="F166">
-            <v>356</v>
-          </cell>
+          <cell r="C166"/>
+          <cell r="D166"/>
+          <cell r="E166"/>
+          <cell r="G166"/>
+          <cell r="H166"/>
         </row>
         <row r="170">
-          <cell r="B170" t="str">
-            <v>Total cost of diesel issued in Week (46)</v>
-          </cell>
-          <cell r="F170">
-            <v>946288</v>
-          </cell>
+          <cell r="C170"/>
+          <cell r="D170"/>
+          <cell r="E170"/>
+          <cell r="G170"/>
+          <cell r="H170"/>
         </row>
         <row r="171">
-          <cell r="B171" t="str">
-            <v>Total cost of diesel issued in Week (47)</v>
-          </cell>
-          <cell r="F171">
-            <v>785497</v>
-          </cell>
+          <cell r="C171"/>
+          <cell r="D171"/>
+          <cell r="E171"/>
+          <cell r="G171"/>
+          <cell r="H171"/>
         </row>
       </sheetData>
       <sheetData sheetId="47">
@@ -5697,88 +5733,120 @@
           <cell r="B159" t="str">
             <v>Previous Week (47) Consumption (in Ltrs)</v>
           </cell>
+          <cell r="C159"/>
+          <cell r="D159"/>
+          <cell r="E159"/>
           <cell r="F159">
             <v>5514</v>
           </cell>
+          <cell r="G159"/>
+          <cell r="H159"/>
         </row>
         <row r="160">
           <cell r="B160" t="str">
             <v>Previous Week (48) Consumption (in Ltrs)</v>
           </cell>
+          <cell r="C160"/>
+          <cell r="D160"/>
+          <cell r="E160"/>
           <cell r="F160">
             <v>5986</v>
           </cell>
+          <cell r="G160"/>
+          <cell r="H160"/>
         </row>
         <row r="162">
           <cell r="B162" t="str">
             <v>Estimated Spillage while Refuelling (in Ltrs)</v>
           </cell>
+          <cell r="C162"/>
+          <cell r="D162"/>
+          <cell r="E162"/>
           <cell r="F162" t="str">
             <v>-</v>
           </cell>
+          <cell r="G162"/>
+          <cell r="H162"/>
         </row>
         <row r="163">
           <cell r="B163" t="str">
             <v>Estmated Leakages in GSE (in Ltrs)</v>
           </cell>
+          <cell r="C163"/>
+          <cell r="D163"/>
+          <cell r="E163"/>
           <cell r="F163" t="str">
             <v>-</v>
           </cell>
+          <cell r="G163"/>
+          <cell r="H163"/>
         </row>
         <row r="164">
           <cell r="B164" t="str">
             <v>Fuel Wasted (in Ltrs)</v>
           </cell>
+          <cell r="C164"/>
+          <cell r="D164"/>
+          <cell r="E164"/>
           <cell r="F164" t="str">
             <v>-</v>
           </cell>
+          <cell r="G164"/>
+          <cell r="H164"/>
         </row>
         <row r="165">
           <cell r="B165" t="str">
             <v>Total number of flights handled in Week (47)</v>
           </cell>
+          <cell r="C165"/>
+          <cell r="D165"/>
+          <cell r="E165"/>
           <cell r="F165">
             <v>349</v>
           </cell>
+          <cell r="G165"/>
+          <cell r="H165"/>
         </row>
         <row r="166">
           <cell r="B166" t="str">
             <v>Total number of flights handled in Week (48)</v>
           </cell>
+          <cell r="C166"/>
+          <cell r="D166"/>
+          <cell r="E166"/>
           <cell r="F166">
             <v>349</v>
           </cell>
+          <cell r="G166"/>
+          <cell r="H166"/>
         </row>
         <row r="170">
           <cell r="B170" t="str">
             <v>Total cost of diesel issued in Week (47)</v>
           </cell>
+          <cell r="C170"/>
+          <cell r="D170"/>
+          <cell r="E170"/>
           <cell r="F170">
             <v>785497</v>
           </cell>
+          <cell r="G170"/>
+          <cell r="H170"/>
         </row>
         <row r="171">
           <cell r="B171" t="str">
             <v>Total cost of diesel issued in Week (48)</v>
           </cell>
+          <cell r="C171"/>
+          <cell r="D171"/>
+          <cell r="E171"/>
           <cell r="F171">
             <v>855998</v>
           </cell>
+          <cell r="G171"/>
+          <cell r="H171"/>
         </row>
       </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="48 (2)"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6139,52 +6207,52 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="206" t="s">
+      <c r="H7" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="206"/>
+      <c r="I7" s="218"/>
     </row>
     <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="207" t="s">
+      <c r="A8" s="219" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="209" t="s">
+      <c r="B8" s="221" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="207" t="s">
+      <c r="C8" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="207" t="s">
+      <c r="D8" s="219" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="207" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="211" t="s">
+      <c r="E8" s="219" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="223" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="211"/>
-      <c r="H8" s="209" t="s">
+      <c r="G8" s="223"/>
+      <c r="H8" s="221" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="209" t="s">
+      <c r="I8" s="221" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="208"/>
-      <c r="B9" s="210"/>
-      <c r="C9" s="208"/>
-      <c r="D9" s="208"/>
-      <c r="E9" s="208"/>
+      <c r="A9" s="220"/>
+      <c r="B9" s="222"/>
+      <c r="C9" s="220"/>
+      <c r="D9" s="220"/>
+      <c r="E9" s="220"/>
       <c r="F9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="210"/>
-      <c r="I9" s="210"/>
+      <c r="H9" s="222"/>
+      <c r="I9" s="222"/>
     </row>
     <row r="10" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
@@ -6226,41 +6294,41 @@
       <c r="I12" s="30"/>
     </row>
     <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="205" t="s">
+      <c r="A13" s="217" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="205"/>
-      <c r="C13" s="205"/>
-      <c r="D13" s="205"/>
-      <c r="E13" s="205"/>
-      <c r="F13" s="205"/>
-      <c r="G13" s="205"/>
-      <c r="H13" s="205"/>
+      <c r="B13" s="217"/>
+      <c r="C13" s="217"/>
+      <c r="D13" s="217"/>
+      <c r="E13" s="217"/>
+      <c r="F13" s="217"/>
+      <c r="G13" s="217"/>
+      <c r="H13" s="217"/>
       <c r="I13" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="197"/>
-      <c r="B14" s="198"/>
-      <c r="C14" s="198"/>
-      <c r="D14" s="198"/>
-      <c r="E14" s="198"/>
-      <c r="F14" s="198"/>
-      <c r="G14" s="198"/>
-      <c r="H14" s="199"/>
-      <c r="I14" s="203"/>
+      <c r="A14" s="209"/>
+      <c r="B14" s="210"/>
+      <c r="C14" s="210"/>
+      <c r="D14" s="210"/>
+      <c r="E14" s="210"/>
+      <c r="F14" s="210"/>
+      <c r="G14" s="210"/>
+      <c r="H14" s="211"/>
+      <c r="I14" s="215"/>
     </row>
     <row r="15" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="200"/>
-      <c r="B15" s="201"/>
-      <c r="C15" s="201"/>
-      <c r="D15" s="201"/>
-      <c r="E15" s="201"/>
-      <c r="F15" s="201"/>
-      <c r="G15" s="201"/>
-      <c r="H15" s="202"/>
-      <c r="I15" s="204"/>
+      <c r="A15" s="212"/>
+      <c r="B15" s="213"/>
+      <c r="C15" s="213"/>
+      <c r="D15" s="213"/>
+      <c r="E15" s="213"/>
+      <c r="F15" s="213"/>
+      <c r="G15" s="213"/>
+      <c r="H15" s="214"/>
+      <c r="I15" s="216"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
@@ -6382,48 +6450,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="228" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
-      <c r="J1" s="224"/>
+      <c r="B1" s="229"/>
+      <c r="C1" s="229"/>
+      <c r="D1" s="229"/>
+      <c r="E1" s="229"/>
+      <c r="F1" s="229"/>
+      <c r="G1" s="229"/>
+      <c r="H1" s="229"/>
+      <c r="I1" s="229"/>
+      <c r="J1" s="229"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="229" t="s">
+      <c r="A2" s="235" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="230"/>
-      <c r="C2" s="230"/>
-      <c r="D2" s="230"/>
-      <c r="E2" s="230"/>
-      <c r="F2" s="230"/>
-      <c r="G2" s="230"/>
-      <c r="H2" s="230"/>
-      <c r="I2" s="230"/>
-      <c r="J2" s="230"/>
+      <c r="B2" s="236"/>
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="236"/>
+      <c r="H2" s="236"/>
+      <c r="I2" s="236"/>
+      <c r="J2" s="236"/>
       <c r="K2" s="38"/>
       <c r="L2" s="72"/>
     </row>
     <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="231" t="s">
+      <c r="A3" s="237" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="232"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="232"/>
-      <c r="F3" s="232"/>
-      <c r="G3" s="232"/>
-      <c r="H3" s="232"/>
-      <c r="I3" s="232"/>
-      <c r="J3" s="232"/>
+      <c r="B3" s="238"/>
+      <c r="C3" s="238"/>
+      <c r="D3" s="238"/>
+      <c r="E3" s="238"/>
+      <c r="F3" s="238"/>
+      <c r="G3" s="238"/>
+      <c r="H3" s="238"/>
+      <c r="I3" s="238"/>
+      <c r="J3" s="238"/>
       <c r="K3" s="73"/>
       <c r="L3" s="127" t="s">
         <v>73</v>
@@ -6737,29 +6805,29 @@
       <c r="K23" s="34"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="226" t="s">
+      <c r="A24" s="232" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="216"/>
+      <c r="B24" s="226"/>
       <c r="C24" s="44"/>
       <c r="D24" s="21"/>
-      <c r="J24" s="217" t="s">
+      <c r="J24" s="224" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="215"/>
-      <c r="L24" s="216"/>
+      <c r="K24" s="225"/>
+      <c r="L24" s="226"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="217" t="s">
+      <c r="A25" s="224" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="216"/>
+      <c r="B25" s="226"/>
       <c r="C25" s="52"/>
       <c r="D25" s="39"/>
-      <c r="E25" s="217" t="s">
+      <c r="E25" s="224" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="216"/>
+      <c r="F25" s="226"/>
       <c r="G25" s="44"/>
       <c r="H25" s="51" t="s">
         <v>75</v>
@@ -6767,40 +6835,40 @@
       <c r="J25" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="217" t="s">
+      <c r="K25" s="224" t="s">
         <v>36</v>
       </c>
-      <c r="L25" s="216"/>
-      <c r="M25" s="212"/>
-      <c r="N25" s="213"/>
-      <c r="O25" s="212"/>
-      <c r="P25" s="213"/>
-      <c r="Q25" s="213"/>
+      <c r="L25" s="226"/>
+      <c r="M25" s="241"/>
+      <c r="N25" s="242"/>
+      <c r="O25" s="241"/>
+      <c r="P25" s="242"/>
+      <c r="Q25" s="242"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="222" t="s">
+      <c r="A26" s="227" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="216"/>
+      <c r="B26" s="226"/>
       <c r="C26" s="49"/>
       <c r="D26" s="48"/>
-      <c r="E26" s="226" t="s">
+      <c r="E26" s="232" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="216"/>
+      <c r="F26" s="226"/>
       <c r="G26" s="47">
         <v>1</v>
       </c>
       <c r="H26" s="46"/>
       <c r="J26" s="45"/>
-      <c r="K26" s="227"/>
-      <c r="L26" s="228"/>
+      <c r="K26" s="233"/>
+      <c r="L26" s="234"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="217" t="s">
+      <c r="A27" s="224" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="216"/>
+      <c r="B27" s="226"/>
       <c r="C27" s="43"/>
       <c r="D27" s="39"/>
       <c r="E27" s="1"/>
@@ -6808,8 +6876,8 @@
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
       <c r="J27" s="42"/>
-      <c r="K27" s="218"/>
-      <c r="L27" s="219"/>
+      <c r="K27" s="243"/>
+      <c r="L27" s="244"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
@@ -6830,72 +6898,72 @@
       <c r="I29" s="32"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="225" t="s">
+      <c r="A30" s="231" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="215"/>
-      <c r="C30" s="216"/>
-      <c r="D30" s="221" t="s">
+      <c r="B30" s="225"/>
+      <c r="C30" s="226"/>
+      <c r="D30" s="230" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="215"/>
-      <c r="F30" s="215"/>
-      <c r="G30" s="216"/>
-      <c r="H30" s="221" t="s">
+      <c r="E30" s="225"/>
+      <c r="F30" s="225"/>
+      <c r="G30" s="226"/>
+      <c r="H30" s="230" t="s">
         <v>30</v>
       </c>
-      <c r="I30" s="221"/>
-      <c r="J30" s="221"/>
+      <c r="I30" s="230"/>
+      <c r="J30" s="230"/>
       <c r="K30" s="50" t="s">
         <v>29</v>
       </c>
       <c r="L30" s="128"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="214"/>
-      <c r="B31" s="215"/>
-      <c r="C31" s="216"/>
-      <c r="D31" s="214"/>
-      <c r="E31" s="215"/>
-      <c r="F31" s="215"/>
-      <c r="G31" s="216"/>
-      <c r="H31" s="214"/>
-      <c r="I31" s="214"/>
-      <c r="J31" s="214"/>
+      <c r="A31" s="239"/>
+      <c r="B31" s="225"/>
+      <c r="C31" s="226"/>
+      <c r="D31" s="239"/>
+      <c r="E31" s="225"/>
+      <c r="F31" s="225"/>
+      <c r="G31" s="226"/>
+      <c r="H31" s="239"/>
+      <c r="I31" s="239"/>
+      <c r="J31" s="239"/>
       <c r="K31" s="129"/>
       <c r="L31" s="124"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="214"/>
-      <c r="B32" s="215"/>
-      <c r="C32" s="216"/>
-      <c r="D32" s="214"/>
-      <c r="E32" s="215"/>
-      <c r="F32" s="215"/>
-      <c r="G32" s="216"/>
-      <c r="H32" s="214"/>
-      <c r="I32" s="214"/>
-      <c r="J32" s="214"/>
+      <c r="A32" s="239"/>
+      <c r="B32" s="225"/>
+      <c r="C32" s="226"/>
+      <c r="D32" s="239"/>
+      <c r="E32" s="225"/>
+      <c r="F32" s="225"/>
+      <c r="G32" s="226"/>
+      <c r="H32" s="239"/>
+      <c r="I32" s="239"/>
+      <c r="J32" s="239"/>
       <c r="K32" s="129"/>
       <c r="L32" s="124"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="214" t="s">
+      <c r="A33" s="239" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="215"/>
-      <c r="C33" s="216"/>
-      <c r="D33" s="214" t="s">
+      <c r="B33" s="225"/>
+      <c r="C33" s="226"/>
+      <c r="D33" s="239" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="215"/>
-      <c r="F33" s="215"/>
-      <c r="G33" s="216"/>
-      <c r="H33" s="214" t="s">
+      <c r="E33" s="225"/>
+      <c r="F33" s="225"/>
+      <c r="G33" s="226"/>
+      <c r="H33" s="239" t="s">
         <v>28</v>
       </c>
-      <c r="I33" s="214"/>
-      <c r="J33" s="220"/>
+      <c r="I33" s="239"/>
+      <c r="J33" s="240"/>
       <c r="K33" s="129" t="s">
         <v>28</v>
       </c>
@@ -6903,6 +6971,21 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
     <mergeCell ref="J24:L24"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A25:B25"/>
@@ -6915,21 +6998,6 @@
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="O25:Q25"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="H32:J32"/>
   </mergeCells>
   <pageMargins left="0.23" right="0.17" top="0.64" bottom="0.17" header="0.38" footer="0.17"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -6964,45 +7032,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="247" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="235"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="234"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="234"/>
+      <c r="B1" s="248"/>
+      <c r="C1" s="249"/>
+      <c r="D1" s="248"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
+      <c r="H1" s="248"/>
+      <c r="I1" s="248"/>
+      <c r="J1" s="248"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="238" t="s">
+      <c r="A2" s="252" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="239"/>
-      <c r="C2" s="240"/>
-      <c r="D2" s="239"/>
-      <c r="E2" s="239"/>
-      <c r="F2" s="239"/>
-      <c r="G2" s="239"/>
-      <c r="H2" s="239"/>
-      <c r="I2" s="239"/>
-      <c r="J2" s="239"/>
+      <c r="B2" s="253"/>
+      <c r="C2" s="254"/>
+      <c r="D2" s="253"/>
+      <c r="E2" s="253"/>
+      <c r="F2" s="253"/>
+      <c r="G2" s="253"/>
+      <c r="H2" s="253"/>
+      <c r="I2" s="253"/>
+      <c r="J2" s="253"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="242" t="s">
+      <c r="A3" s="256" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="243"/>
-      <c r="C3" s="243"/>
-      <c r="D3" s="243"/>
-      <c r="E3" s="243"/>
-      <c r="F3" s="243"/>
-      <c r="G3" s="243"/>
-      <c r="H3" s="243"/>
-      <c r="I3" s="243"/>
+      <c r="B3" s="257"/>
+      <c r="C3" s="257"/>
+      <c r="D3" s="257"/>
+      <c r="E3" s="257"/>
+      <c r="F3" s="257"/>
+      <c r="G3" s="257"/>
+      <c r="H3" s="257"/>
+      <c r="I3" s="257"/>
       <c r="J3" s="127" t="s">
         <v>74</v>
       </c>
@@ -7268,12 +7336,12 @@
       <c r="M21" s="108"/>
     </row>
     <row r="22" spans="1:13" s="99" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="244" t="s">
+      <c r="A22" s="258" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="215"/>
-      <c r="C22" s="215"/>
-      <c r="D22" s="216"/>
+      <c r="B22" s="225"/>
+      <c r="C22" s="225"/>
+      <c r="D22" s="226"/>
       <c r="E22" s="106"/>
       <c r="F22" s="43"/>
       <c r="G22" s="105">
@@ -7305,37 +7373,37 @@
       <c r="K23" s="100"/>
     </row>
     <row r="24" spans="1:13" s="99" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="217" t="s">
+      <c r="A24" s="224" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="216"/>
-      <c r="C24" s="237"/>
-      <c r="D24" s="215"/>
-      <c r="E24" s="216"/>
+      <c r="B24" s="226"/>
+      <c r="C24" s="251"/>
+      <c r="D24" s="225"/>
+      <c r="E24" s="226"/>
       <c r="F24" s="38"/>
       <c r="G24" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="236"/>
-      <c r="I24" s="215"/>
-      <c r="J24" s="216"/>
+      <c r="H24" s="250"/>
+      <c r="I24" s="225"/>
+      <c r="J24" s="226"/>
       <c r="K24" s="100"/>
     </row>
     <row r="25" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="217" t="s">
+      <c r="A25" s="224" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="216"/>
-      <c r="C25" s="237"/>
-      <c r="D25" s="215"/>
-      <c r="E25" s="216"/>
+      <c r="B25" s="226"/>
+      <c r="C25" s="251"/>
+      <c r="D25" s="225"/>
+      <c r="E25" s="226"/>
       <c r="F25" s="38"/>
       <c r="G25" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="H25" s="241"/>
-      <c r="I25" s="215"/>
-      <c r="J25" s="216"/>
+      <c r="H25" s="255"/>
+      <c r="I25" s="225"/>
+      <c r="J25" s="226"/>
     </row>
     <row r="26" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="95"/>
@@ -7351,72 +7419,72 @@
       <c r="K26" s="92"/>
     </row>
     <row r="27" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="214" t="s">
+      <c r="A27" s="239" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="216"/>
-      <c r="C27" s="221" t="s">
+      <c r="B27" s="226"/>
+      <c r="C27" s="230" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="216"/>
+      <c r="D27" s="226"/>
       <c r="E27" s="51" t="s">
         <v>30</v>
       </c>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
       <c r="H27" s="94"/>
-      <c r="I27" s="214" t="s">
+      <c r="I27" s="239" t="s">
         <v>29</v>
       </c>
-      <c r="J27" s="216"/>
+      <c r="J27" s="226"/>
       <c r="K27" s="92"/>
       <c r="M27" s="93"/>
     </row>
     <row r="28" spans="1:13" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="214"/>
-      <c r="B28" s="216"/>
-      <c r="C28" s="214"/>
-      <c r="D28" s="216"/>
-      <c r="E28" s="214"/>
-      <c r="F28" s="215"/>
-      <c r="G28" s="215"/>
-      <c r="H28" s="216"/>
-      <c r="I28" s="214"/>
-      <c r="J28" s="216"/>
+      <c r="A28" s="239"/>
+      <c r="B28" s="226"/>
+      <c r="C28" s="239"/>
+      <c r="D28" s="226"/>
+      <c r="E28" s="239"/>
+      <c r="F28" s="225"/>
+      <c r="G28" s="225"/>
+      <c r="H28" s="226"/>
+      <c r="I28" s="239"/>
+      <c r="J28" s="226"/>
       <c r="K28" s="92"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="214"/>
-      <c r="B29" s="216"/>
-      <c r="C29" s="214"/>
-      <c r="D29" s="216"/>
-      <c r="E29" s="214"/>
-      <c r="F29" s="215"/>
-      <c r="G29" s="215"/>
-      <c r="H29" s="216"/>
-      <c r="I29" s="214"/>
-      <c r="J29" s="216"/>
+      <c r="A29" s="239"/>
+      <c r="B29" s="226"/>
+      <c r="C29" s="239"/>
+      <c r="D29" s="226"/>
+      <c r="E29" s="239"/>
+      <c r="F29" s="225"/>
+      <c r="G29" s="225"/>
+      <c r="H29" s="226"/>
+      <c r="I29" s="239"/>
+      <c r="J29" s="226"/>
       <c r="L29" s="90"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="214" t="s">
+      <c r="A30" s="239" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="216"/>
-      <c r="C30" s="214" t="s">
+      <c r="B30" s="226"/>
+      <c r="C30" s="239" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="216"/>
-      <c r="E30" s="214" t="s">
+      <c r="D30" s="226"/>
+      <c r="E30" s="239" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="215"/>
-      <c r="G30" s="215"/>
-      <c r="H30" s="216"/>
-      <c r="I30" s="214" t="s">
+      <c r="F30" s="225"/>
+      <c r="G30" s="225"/>
+      <c r="H30" s="226"/>
+      <c r="I30" s="239" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="216"/>
+      <c r="J30" s="226"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
@@ -7492,6 +7560,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="I27:J27"/>
     <mergeCell ref="G35:H35"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="A29:B29"/>
@@ -7505,19 +7586,6 @@
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="I27:J27"/>
   </mergeCells>
   <pageMargins left="0.18" right="0.17" top="0.72" bottom="0.17" header="0.3" footer="0.17"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -7687,10 +7755,10 @@
       <c r="K10" s="152"/>
     </row>
     <row r="11" spans="1:11" ht="12" x14ac:dyDescent="0.25">
-      <c r="A11" s="247" t="s">
+      <c r="A11" s="259" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="248"/>
+      <c r="B11" s="260"/>
       <c r="C11" s="153" t="s">
         <v>89</v>
       </c>
@@ -7791,42 +7859,42 @@
       <c r="K16" s="166"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="249" t="s">
+      <c r="A17" s="261" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="250"/>
-      <c r="C17" s="250"/>
-      <c r="D17" s="250"/>
-      <c r="E17" s="250"/>
-      <c r="F17" s="250"/>
-      <c r="G17" s="250"/>
-      <c r="H17" s="250"/>
-      <c r="I17" s="250"/>
-      <c r="J17" s="250"/>
-      <c r="K17" s="251"/>
+      <c r="B17" s="262"/>
+      <c r="C17" s="262"/>
+      <c r="D17" s="262"/>
+      <c r="E17" s="262"/>
+      <c r="F17" s="262"/>
+      <c r="G17" s="262"/>
+      <c r="H17" s="262"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="262"/>
+      <c r="K17" s="263"/>
     </row>
     <row r="18" spans="1:11" ht="12" x14ac:dyDescent="0.25">
-      <c r="A18" s="252" t="s">
+      <c r="A18" s="264" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="253"/>
-      <c r="C18" s="253"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="255" t="s">
+      <c r="B18" s="265"/>
+      <c r="C18" s="265"/>
+      <c r="D18" s="266"/>
+      <c r="E18" s="267" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="255"/>
-      <c r="G18" s="255"/>
-      <c r="H18" s="256" t="s">
+      <c r="F18" s="267"/>
+      <c r="G18" s="267"/>
+      <c r="H18" s="268" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="256" t="s">
+      <c r="I18" s="268" t="s">
         <v>103</v>
       </c>
-      <c r="J18" s="256" t="s">
+      <c r="J18" s="268" t="s">
         <v>104</v>
       </c>
-      <c r="K18" s="255" t="s">
+      <c r="K18" s="267" t="s">
         <v>18</v>
       </c>
     </row>
@@ -7852,10 +7920,10 @@
       <c r="G19" s="169" t="s">
         <v>108</v>
       </c>
-      <c r="H19" s="256"/>
-      <c r="I19" s="256"/>
-      <c r="J19" s="256"/>
-      <c r="K19" s="255"/>
+      <c r="H19" s="268"/>
+      <c r="I19" s="268"/>
+      <c r="J19" s="268"/>
+      <c r="K19" s="267"/>
     </row>
     <row r="20" spans="1:11" ht="12" x14ac:dyDescent="0.25">
       <c r="A20" s="168"/>
@@ -8878,98 +8946,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B44655-1AD6-4F0D-BE2C-CEF7A76DFF02}">
   <dimension ref="A1:S191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="T174" sqref="T174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="34" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="176" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="34" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="34" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="34" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="34" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="34" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="34" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" style="34" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="34" customWidth="1"/>
+    <col min="9" max="9" width="7" style="34" customWidth="1"/>
     <col min="10" max="10" width="7.28515625" style="34" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" style="34" customWidth="1"/>
+    <col min="11" max="11" width="7" style="34" customWidth="1"/>
     <col min="12" max="12" width="7.28515625" style="34" customWidth="1"/>
     <col min="13" max="13" width="6.7109375" style="34" customWidth="1"/>
-    <col min="14" max="14" width="7.28515625" style="34" customWidth="1"/>
+    <col min="14" max="14" width="7.5703125" style="34" customWidth="1"/>
     <col min="15" max="15" width="6.7109375" style="34" customWidth="1"/>
-    <col min="16" max="16" width="7" style="34" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="34" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" style="34" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" style="34" customWidth="1"/>
     <col min="18" max="18" width="14.42578125" style="34" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="282" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="265"/>
-      <c r="C1" s="268"/>
-      <c r="D1" s="268"/>
-      <c r="E1" s="268"/>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="268"/>
-      <c r="M1" s="268"/>
-      <c r="N1" s="268"/>
-      <c r="O1" s="268"/>
-      <c r="P1" s="268"/>
-      <c r="Q1" s="268"/>
-      <c r="R1" s="268"/>
+      <c r="B1" s="282"/>
+      <c r="C1" s="283"/>
+      <c r="D1" s="283"/>
+      <c r="E1" s="283"/>
+      <c r="F1" s="283"/>
+      <c r="G1" s="283"/>
+      <c r="H1" s="283"/>
+      <c r="I1" s="283"/>
+      <c r="J1" s="283"/>
+      <c r="K1" s="283"/>
+      <c r="L1" s="283"/>
+      <c r="M1" s="283"/>
+      <c r="N1" s="283"/>
+      <c r="O1" s="283"/>
+      <c r="P1" s="283"/>
+      <c r="Q1" s="283"/>
+      <c r="R1" s="283"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="265" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" s="265"/>
-      <c r="C2" s="268"/>
-      <c r="D2" s="268"/>
-      <c r="E2" s="268"/>
-      <c r="F2" s="268"/>
-      <c r="G2" s="268"/>
-      <c r="H2" s="268"/>
-      <c r="I2" s="268"/>
-      <c r="J2" s="268"/>
-      <c r="K2" s="268"/>
-      <c r="L2" s="268"/>
-      <c r="M2" s="268"/>
-      <c r="N2" s="268"/>
-      <c r="O2" s="268"/>
-      <c r="P2" s="268"/>
-      <c r="Q2" s="268"/>
-      <c r="R2" s="268"/>
+      <c r="A2" s="282" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="282"/>
+      <c r="C2" s="283"/>
+      <c r="D2" s="283"/>
+      <c r="E2" s="283"/>
+      <c r="F2" s="283"/>
+      <c r="G2" s="283"/>
+      <c r="H2" s="283"/>
+      <c r="I2" s="283"/>
+      <c r="J2" s="283"/>
+      <c r="K2" s="283"/>
+      <c r="L2" s="283"/>
+      <c r="M2" s="283"/>
+      <c r="N2" s="283"/>
+      <c r="O2" s="283"/>
+      <c r="P2" s="283"/>
+      <c r="Q2" s="283"/>
+      <c r="R2" s="283"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="278" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="265"/>
-      <c r="C3" s="268"/>
-      <c r="D3" s="268"/>
-      <c r="E3" s="268"/>
-      <c r="F3" s="268"/>
-      <c r="G3" s="268"/>
-      <c r="H3" s="268"/>
-      <c r="I3" s="268"/>
-      <c r="J3" s="268"/>
-      <c r="K3" s="268"/>
-      <c r="L3" s="268"/>
-      <c r="M3" s="268"/>
-      <c r="N3" s="268"/>
-      <c r="O3" s="268"/>
-      <c r="P3" s="268"/>
-      <c r="Q3" s="268"/>
-      <c r="R3" s="268"/>
+      <c r="A3" s="284" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="282"/>
+      <c r="C3" s="283"/>
+      <c r="D3" s="283"/>
+      <c r="E3" s="283"/>
+      <c r="F3" s="283"/>
+      <c r="G3" s="283"/>
+      <c r="H3" s="283"/>
+      <c r="I3" s="283"/>
+      <c r="J3" s="283"/>
+      <c r="K3" s="283"/>
+      <c r="L3" s="283"/>
+      <c r="M3" s="283"/>
+      <c r="N3" s="283"/>
+      <c r="O3" s="283"/>
+      <c r="P3" s="283"/>
+      <c r="Q3" s="283"/>
+      <c r="R3" s="283"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -9027,81 +9095,79 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="P6" s="269" t="s">
+      <c r="P6" s="285" t="s">
         <v>81</v>
       </c>
-      <c r="Q6" s="259"/>
+      <c r="Q6" s="270"/>
       <c r="R6" s="182"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="270" t="s">
+      <c r="A7" s="286" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="228"/>
-      <c r="C7" s="264"/>
-      <c r="D7" s="228"/>
-      <c r="E7" s="264"/>
-      <c r="F7" s="228"/>
-      <c r="G7" s="264"/>
-      <c r="H7" s="228"/>
-      <c r="I7" s="264"/>
-      <c r="J7" s="228"/>
-      <c r="K7" s="264"/>
-      <c r="L7" s="228"/>
-      <c r="M7" s="264"/>
-      <c r="N7" s="228"/>
-      <c r="O7" s="264"/>
-      <c r="P7" s="228"/>
-      <c r="Q7" s="264" t="s">
+      <c r="B7" s="234"/>
+      <c r="C7" s="277"/>
+      <c r="D7" s="234"/>
+      <c r="E7" s="277"/>
+      <c r="F7" s="234"/>
+      <c r="G7" s="277"/>
+      <c r="H7" s="234"/>
+      <c r="I7" s="277"/>
+      <c r="J7" s="234"/>
+      <c r="K7" s="277"/>
+      <c r="L7" s="234"/>
+      <c r="M7" s="277"/>
+      <c r="N7" s="234"/>
+      <c r="O7" s="277"/>
+      <c r="P7" s="234"/>
+      <c r="Q7" s="277" t="s">
         <v>114</v>
       </c>
-      <c r="R7" s="264" t="s">
+      <c r="R7" s="277" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="271"/>
-      <c r="B8" s="219"/>
-      <c r="C8" s="271"/>
-      <c r="D8" s="219"/>
-      <c r="E8" s="271"/>
-      <c r="F8" s="219"/>
-      <c r="G8" s="271"/>
-      <c r="H8" s="219"/>
-      <c r="I8" s="271"/>
-      <c r="J8" s="219"/>
-      <c r="K8" s="271"/>
-      <c r="L8" s="219"/>
-      <c r="M8" s="271"/>
-      <c r="N8" s="219"/>
-      <c r="O8" s="271"/>
-      <c r="P8" s="219"/>
-      <c r="Q8" s="272"/>
-      <c r="R8" s="272"/>
+      <c r="A8" s="287"/>
+      <c r="B8" s="244"/>
+      <c r="C8" s="287"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="287"/>
+      <c r="F8" s="244"/>
+      <c r="G8" s="287"/>
+      <c r="H8" s="244"/>
+      <c r="I8" s="287"/>
+      <c r="J8" s="244"/>
+      <c r="K8" s="287"/>
+      <c r="L8" s="244"/>
+      <c r="M8" s="287"/>
+      <c r="N8" s="244"/>
+      <c r="O8" s="287"/>
+      <c r="P8" s="244"/>
+      <c r="Q8" s="288"/>
+      <c r="R8" s="288"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="270" t="s">
+      <c r="A9" s="286" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="216"/>
-      <c r="C9" s="264">
-        <v>142</v>
-      </c>
-      <c r="D9" s="216"/>
-      <c r="E9" s="264"/>
-      <c r="F9" s="216"/>
-      <c r="G9" s="264"/>
-      <c r="H9" s="216"/>
-      <c r="I9" s="264"/>
-      <c r="J9" s="216"/>
-      <c r="K9" s="264"/>
-      <c r="L9" s="216"/>
-      <c r="M9" s="264"/>
-      <c r="N9" s="216"/>
-      <c r="O9" s="264"/>
-      <c r="P9" s="216"/>
-      <c r="Q9" s="272"/>
-      <c r="R9" s="272"/>
+      <c r="B9" s="226"/>
+      <c r="C9" s="277"/>
+      <c r="D9" s="226"/>
+      <c r="E9" s="277"/>
+      <c r="F9" s="226"/>
+      <c r="G9" s="277"/>
+      <c r="H9" s="226"/>
+      <c r="I9" s="277"/>
+      <c r="J9" s="226"/>
+      <c r="K9" s="277"/>
+      <c r="L9" s="226"/>
+      <c r="M9" s="277"/>
+      <c r="N9" s="226"/>
+      <c r="O9" s="277"/>
+      <c r="P9" s="226"/>
+      <c r="Q9" s="288"/>
+      <c r="R9" s="288"/>
     </row>
     <row r="10" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
@@ -9152,8 +9218,8 @@
       <c r="P10" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="Q10" s="273"/>
-      <c r="R10" s="273"/>
+      <c r="Q10" s="289"/>
+      <c r="R10" s="289"/>
     </row>
     <row r="11" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94">
@@ -9189,7 +9255,7 @@
       <c r="A12" s="94">
         <v>2</v>
       </c>
-      <c r="B12" s="274">
+      <c r="B12" s="197">
         <v>110</v>
       </c>
       <c r="C12" s="57"/>
@@ -9219,7 +9285,7 @@
       <c r="A13" s="94">
         <v>3</v>
       </c>
-      <c r="B13" s="274">
+      <c r="B13" s="197">
         <v>112</v>
       </c>
       <c r="C13" s="57"/>
@@ -9249,7 +9315,7 @@
       <c r="A14" s="94">
         <v>4</v>
       </c>
-      <c r="B14" s="274">
+      <c r="B14" s="197">
         <v>113</v>
       </c>
       <c r="C14" s="57"/>
@@ -9279,7 +9345,7 @@
       <c r="A15" s="94">
         <v>6</v>
       </c>
-      <c r="B15" s="274">
+      <c r="B15" s="197">
         <v>115</v>
       </c>
       <c r="C15" s="57"/>
@@ -9309,7 +9375,7 @@
       <c r="A16" s="94">
         <v>7</v>
       </c>
-      <c r="B16" s="274">
+      <c r="B16" s="197">
         <v>116</v>
       </c>
       <c r="C16" s="57"/>
@@ -9339,7 +9405,7 @@
       <c r="A17" s="94">
         <v>8</v>
       </c>
-      <c r="B17" s="274">
+      <c r="B17" s="197">
         <v>117</v>
       </c>
       <c r="C17" s="57"/>
@@ -9369,7 +9435,7 @@
       <c r="A18" s="94">
         <v>9</v>
       </c>
-      <c r="B18" s="274">
+      <c r="B18" s="197">
         <v>118</v>
       </c>
       <c r="C18" s="57"/>
@@ -9399,7 +9465,7 @@
       <c r="A19" s="94">
         <v>10</v>
       </c>
-      <c r="B19" s="274">
+      <c r="B19" s="197">
         <v>201</v>
       </c>
       <c r="C19" s="57"/>
@@ -9429,7 +9495,7 @@
       <c r="A20" s="94">
         <v>11</v>
       </c>
-      <c r="B20" s="274">
+      <c r="B20" s="197">
         <v>204</v>
       </c>
       <c r="C20" s="57"/>
@@ -9459,8 +9525,8 @@
       <c r="A21" s="94">
         <v>12</v>
       </c>
-      <c r="B21" s="274" t="s">
-        <v>142</v>
+      <c r="B21" s="197" t="s">
+        <v>133</v>
       </c>
       <c r="C21" s="57"/>
       <c r="D21" s="57"/>
@@ -9489,7 +9555,7 @@
       <c r="A22" s="94">
         <v>13</v>
       </c>
-      <c r="B22" s="274">
+      <c r="B22" s="197">
         <v>327</v>
       </c>
       <c r="C22" s="57"/>
@@ -9519,7 +9585,7 @@
       <c r="A23" s="94">
         <v>14</v>
       </c>
-      <c r="B23" s="274">
+      <c r="B23" s="197">
         <v>328</v>
       </c>
       <c r="C23" s="57"/>
@@ -9549,7 +9615,7 @@
       <c r="A24" s="94">
         <v>15</v>
       </c>
-      <c r="B24" s="274">
+      <c r="B24" s="197">
         <v>329</v>
       </c>
       <c r="C24" s="57"/>
@@ -9579,7 +9645,7 @@
       <c r="A25" s="94">
         <v>16</v>
       </c>
-      <c r="B25" s="274">
+      <c r="B25" s="197">
         <v>330</v>
       </c>
       <c r="C25" s="57"/>
@@ -9609,7 +9675,7 @@
       <c r="A26" s="94">
         <v>17</v>
       </c>
-      <c r="B26" s="274">
+      <c r="B26" s="197">
         <v>331</v>
       </c>
       <c r="C26" s="57"/>
@@ -9639,7 +9705,7 @@
       <c r="A27" s="94">
         <v>18</v>
       </c>
-      <c r="B27" s="274">
+      <c r="B27" s="197">
         <v>332</v>
       </c>
       <c r="C27" s="57"/>
@@ -9669,7 +9735,7 @@
       <c r="A28" s="94">
         <v>19</v>
       </c>
-      <c r="B28" s="274">
+      <c r="B28" s="197">
         <v>333</v>
       </c>
       <c r="C28" s="57"/>
@@ -9699,7 +9765,7 @@
       <c r="A29" s="94">
         <v>20</v>
       </c>
-      <c r="B29" s="274">
+      <c r="B29" s="197">
         <v>334</v>
       </c>
       <c r="C29" s="57"/>
@@ -9729,7 +9795,7 @@
       <c r="A30" s="94">
         <v>22</v>
       </c>
-      <c r="B30" s="274">
+      <c r="B30" s="197">
         <v>336</v>
       </c>
       <c r="C30" s="57"/>
@@ -9759,7 +9825,7 @@
       <c r="A31" s="94">
         <v>24</v>
       </c>
-      <c r="B31" s="274">
+      <c r="B31" s="197">
         <v>338</v>
       </c>
       <c r="C31" s="57"/>
@@ -9879,7 +9945,7 @@
       <c r="A35" s="94">
         <v>28</v>
       </c>
-      <c r="B35" s="275">
+      <c r="B35" s="198">
         <v>342</v>
       </c>
       <c r="C35" s="57"/>
@@ -9939,8 +10005,8 @@
       <c r="A37" s="94">
         <v>30</v>
       </c>
-      <c r="B37" s="274" t="s">
-        <v>143</v>
+      <c r="B37" s="197" t="s">
+        <v>134</v>
       </c>
       <c r="C37" s="57"/>
       <c r="D37" s="57"/>
@@ -9969,8 +10035,8 @@
       <c r="A38" s="94">
         <v>31</v>
       </c>
-      <c r="B38" s="274" t="s">
-        <v>144</v>
+      <c r="B38" s="197" t="s">
+        <v>135</v>
       </c>
       <c r="C38" s="57"/>
       <c r="D38" s="57"/>
@@ -9999,8 +10065,8 @@
       <c r="A39" s="94">
         <v>32</v>
       </c>
-      <c r="B39" s="274" t="s">
-        <v>145</v>
+      <c r="B39" s="197" t="s">
+        <v>136</v>
       </c>
       <c r="C39" s="57"/>
       <c r="D39" s="57"/>
@@ -10029,7 +10095,7 @@
       <c r="A40" s="94">
         <v>33</v>
       </c>
-      <c r="B40" s="274">
+      <c r="B40" s="197">
         <v>417</v>
       </c>
       <c r="C40" s="57"/>
@@ -10089,7 +10155,7 @@
       <c r="A42" s="94">
         <v>37</v>
       </c>
-      <c r="B42" s="274">
+      <c r="B42" s="197">
         <v>421</v>
       </c>
       <c r="C42" s="57"/>
@@ -10750,7 +10816,7 @@
         <v>60</v>
       </c>
       <c r="B64" s="187" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C64" s="57"/>
       <c r="D64" s="57"/>
@@ -11135,11 +11201,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:18" s="277" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" s="200" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="94">
         <v>74</v>
       </c>
-      <c r="B77" s="276">
+      <c r="B77" s="199">
         <v>618</v>
       </c>
       <c r="C77" s="57"/>
@@ -11560,7 +11626,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="187" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C91" s="57"/>
       <c r="D91" s="57"/>
@@ -12520,7 +12586,7 @@
         <v>127</v>
       </c>
       <c r="B123" s="187" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C123" s="57"/>
       <c r="D123" s="57"/>
@@ -12790,7 +12856,7 @@
         <v>136</v>
       </c>
       <c r="B132" s="187" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C132" s="57"/>
       <c r="D132" s="57"/>
@@ -13300,7 +13366,7 @@
         <v>154</v>
       </c>
       <c r="B149" s="187" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C149" s="57"/>
       <c r="D149" s="57"/>
@@ -13330,7 +13396,7 @@
         <v>155</v>
       </c>
       <c r="B150" s="187" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C150" s="57"/>
       <c r="D150" s="57"/>
@@ -13360,7 +13426,7 @@
         <v>156</v>
       </c>
       <c r="B151" s="187" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C151" s="57"/>
       <c r="D151" s="57"/>
@@ -13390,7 +13456,7 @@
         <v>157</v>
       </c>
       <c r="B152" s="187" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C152" s="57"/>
       <c r="D152" s="57"/>
@@ -13416,22 +13482,22 @@
       </c>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A153" s="262"/>
-      <c r="B153" s="215"/>
-      <c r="C153" s="215"/>
-      <c r="D153" s="215"/>
-      <c r="E153" s="215"/>
-      <c r="F153" s="215"/>
-      <c r="G153" s="215"/>
-      <c r="H153" s="215"/>
-      <c r="I153" s="215"/>
-      <c r="J153" s="215"/>
-      <c r="K153" s="215"/>
-      <c r="L153" s="215"/>
-      <c r="M153" s="215"/>
-      <c r="N153" s="215"/>
-      <c r="O153" s="215"/>
-      <c r="P153" s="216"/>
+      <c r="A153" s="273"/>
+      <c r="B153" s="225"/>
+      <c r="C153" s="225"/>
+      <c r="D153" s="225"/>
+      <c r="E153" s="225"/>
+      <c r="F153" s="225"/>
+      <c r="G153" s="225"/>
+      <c r="H153" s="225"/>
+      <c r="I153" s="225"/>
+      <c r="J153" s="225"/>
+      <c r="K153" s="225"/>
+      <c r="L153" s="225"/>
+      <c r="M153" s="225"/>
+      <c r="N153" s="225"/>
+      <c r="O153" s="225"/>
+      <c r="P153" s="226"/>
       <c r="Q153" s="187">
         <f>SUM(Q11:Q152)</f>
         <v>0</v>
@@ -13442,10 +13508,10 @@
       </c>
     </row>
     <row r="154" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="264" t="s">
+      <c r="A154" s="277" t="s">
         <v>119</v>
       </c>
-      <c r="B154" s="216"/>
+      <c r="B154" s="226"/>
       <c r="C154" s="94">
         <f>SUM(C11:C152)</f>
         <v>0</v>
@@ -13488,10 +13554,10 @@
       <c r="R154" s="190"/>
     </row>
     <row r="155" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="264" t="s">
+      <c r="A155" s="277" t="s">
         <v>120</v>
       </c>
-      <c r="B155" s="216"/>
+      <c r="B155" s="226"/>
       <c r="C155" s="94">
         <f>C154*C9</f>
         <v>0</v>
@@ -13528,7 +13594,7 @@
       </c>
       <c r="P155" s="94"/>
       <c r="Q155" s="94" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="R155" s="191">
         <f>SUM(C155:P155)</f>
@@ -13537,8 +13603,8 @@
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
-      <c r="B156" s="279"/>
-      <c r="C156" s="280"/>
+      <c r="B156" s="278"/>
+      <c r="C156" s="279"/>
       <c r="D156" s="1"/>
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
@@ -13556,471 +13622,401 @@
       <c r="R156" s="1"/>
     </row>
     <row r="157" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="266" t="s">
+      <c r="A157" s="280" t="s">
         <v>121</v>
       </c>
-      <c r="B157" s="259"/>
-      <c r="C157" s="259"/>
-      <c r="D157" s="259"/>
-      <c r="E157" s="259"/>
-      <c r="F157" s="259"/>
-      <c r="G157" s="259"/>
-      <c r="H157" s="259"/>
-      <c r="I157" s="259"/>
-      <c r="J157" s="259"/>
-      <c r="K157" s="259"/>
-      <c r="L157" s="259"/>
-      <c r="M157" s="259"/>
-      <c r="N157" s="259"/>
-      <c r="O157" s="259"/>
-      <c r="P157" s="259"/>
-      <c r="Q157" s="259"/>
+      <c r="B157" s="270"/>
+      <c r="C157" s="270"/>
+      <c r="D157" s="270"/>
+      <c r="E157" s="270"/>
+      <c r="F157" s="270"/>
+      <c r="G157" s="270"/>
+      <c r="H157" s="270"/>
+      <c r="I157" s="270"/>
+      <c r="J157" s="270"/>
+      <c r="K157" s="270"/>
+      <c r="L157" s="270"/>
+      <c r="M157" s="270"/>
+      <c r="N157" s="270"/>
+      <c r="O157" s="270"/>
+      <c r="P157" s="270"/>
+      <c r="Q157" s="270"/>
       <c r="R157" s="1"/>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="189" t="s">
         <v>122</v>
       </c>
-      <c r="B158" s="257" t="s">
+      <c r="B158" s="275" t="s">
         <v>123</v>
       </c>
-      <c r="C158" s="215"/>
-      <c r="D158" s="215"/>
-      <c r="E158" s="215"/>
-      <c r="F158" s="215"/>
-      <c r="G158" s="215"/>
-      <c r="H158" s="215"/>
-      <c r="I158" s="215"/>
-      <c r="J158" s="215"/>
-      <c r="K158" s="215"/>
-      <c r="L158" s="215"/>
-      <c r="M158" s="215"/>
-      <c r="N158" s="215"/>
-      <c r="O158" s="215"/>
-      <c r="P158" s="215"/>
-      <c r="Q158" s="215"/>
-      <c r="R158" s="216"/>
+      <c r="C158" s="225"/>
+      <c r="D158" s="225"/>
+      <c r="E158" s="225"/>
+      <c r="F158" s="225"/>
+      <c r="G158" s="225"/>
+      <c r="H158" s="225"/>
+      <c r="I158" s="225"/>
+      <c r="J158" s="225"/>
+      <c r="K158" s="225"/>
+      <c r="L158" s="225"/>
+      <c r="M158" s="225"/>
+      <c r="N158" s="225"/>
+      <c r="O158" s="225"/>
+      <c r="P158" s="225"/>
+      <c r="Q158" s="225"/>
+      <c r="R158" s="226"/>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="46">
         <v>1</v>
       </c>
-      <c r="B159" s="267" t="str">
-        <f>IFERROR("Previous Week ("&amp;R5-1&amp;") Consumption (in Ltrs)",""-"")</f>
-        <v>Previous Week (-1) Consumption (in Ltrs)</v>
-      </c>
-      <c r="C159" s="259"/>
-      <c r="D159" s="259"/>
-      <c r="E159" s="219"/>
-      <c r="F159" s="258" t="str">
-        <f t="array" aca="1" ref="F159" ca="1">IFERROR(INDIRECT("'" &amp; R5-1 &amp; "'!Q154"),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="G159" s="259"/>
-      <c r="H159" s="219"/>
-      <c r="I159" s="262"/>
-      <c r="J159" s="215"/>
-      <c r="K159" s="215"/>
-      <c r="L159" s="215"/>
-      <c r="M159" s="215"/>
-      <c r="N159" s="215"/>
-      <c r="O159" s="215"/>
-      <c r="P159" s="215"/>
-      <c r="Q159" s="215"/>
-      <c r="R159" s="216"/>
+      <c r="B159" s="281"/>
+      <c r="C159" s="270"/>
+      <c r="D159" s="270"/>
+      <c r="E159" s="244"/>
+      <c r="F159" s="269"/>
+      <c r="G159" s="270"/>
+      <c r="H159" s="244"/>
+      <c r="I159" s="273"/>
+      <c r="J159" s="225"/>
+      <c r="K159" s="225"/>
+      <c r="L159" s="225"/>
+      <c r="M159" s="225"/>
+      <c r="N159" s="225"/>
+      <c r="O159" s="225"/>
+      <c r="P159" s="225"/>
+      <c r="Q159" s="225"/>
+      <c r="R159" s="226"/>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="46">
         <v>2</v>
       </c>
-      <c r="B160" s="260" t="str">
-        <f>IFERROR("Previous Week ("&amp;R5&amp;") Consumption (in Ltrs)",""-"")</f>
-        <v>Previous Week () Consumption (in Ltrs)</v>
-      </c>
-      <c r="C160" s="215"/>
-      <c r="D160" s="215"/>
-      <c r="E160" s="216"/>
-      <c r="F160" s="258" t="str">
-        <f t="array" aca="1" ref="F160" ca="1">IFERROR(INDIRECT("'" &amp; R5 &amp; "'!Q154"),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="G160" s="259"/>
-      <c r="H160" s="219"/>
-      <c r="I160" s="262"/>
-      <c r="J160" s="215"/>
-      <c r="K160" s="215"/>
-      <c r="L160" s="215"/>
-      <c r="M160" s="215"/>
-      <c r="N160" s="215"/>
-      <c r="O160" s="215"/>
-      <c r="P160" s="215"/>
-      <c r="Q160" s="215"/>
-      <c r="R160" s="216"/>
+      <c r="B160" s="271"/>
+      <c r="C160" s="225"/>
+      <c r="D160" s="225"/>
+      <c r="E160" s="226"/>
+      <c r="F160" s="269"/>
+      <c r="G160" s="270"/>
+      <c r="H160" s="244"/>
+      <c r="I160" s="273"/>
+      <c r="J160" s="225"/>
+      <c r="K160" s="225"/>
+      <c r="L160" s="225"/>
+      <c r="M160" s="225"/>
+      <c r="N160" s="225"/>
+      <c r="O160" s="225"/>
+      <c r="P160" s="225"/>
+      <c r="Q160" s="225"/>
+      <c r="R160" s="226"/>
     </row>
     <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" s="46">
         <v>3</v>
       </c>
-      <c r="B161" s="260" t="s">
+      <c r="B161" s="271" t="s">
         <v>124</v>
       </c>
-      <c r="C161" s="215"/>
-      <c r="D161" s="215"/>
-      <c r="E161" s="216"/>
-      <c r="F161" s="258">
-        <f ca="1">IFERROR(F159-F160,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G161" s="259"/>
-      <c r="H161" s="219"/>
-      <c r="I161" s="263" t="str">
-        <f ca="1">IFERROR(
-  IF(F160 - F159 &lt; 0,
-     "Decrease in fuel consumption this week",
-     "Increase in fuel consumption this week"
-  ),
-  "-"
-)</f>
-        <v>-</v>
-      </c>
-      <c r="J161" s="215"/>
-      <c r="K161" s="215"/>
-      <c r="L161" s="215"/>
-      <c r="M161" s="215"/>
-      <c r="N161" s="215"/>
-      <c r="O161" s="215"/>
-      <c r="P161" s="215"/>
-      <c r="Q161" s="215"/>
-      <c r="R161" s="216"/>
+      <c r="C161" s="225"/>
+      <c r="D161" s="225"/>
+      <c r="E161" s="226"/>
+      <c r="F161" s="269"/>
+      <c r="G161" s="270"/>
+      <c r="H161" s="244"/>
+      <c r="I161" s="274"/>
+      <c r="J161" s="225"/>
+      <c r="K161" s="225"/>
+      <c r="L161" s="225"/>
+      <c r="M161" s="225"/>
+      <c r="N161" s="225"/>
+      <c r="O161" s="225"/>
+      <c r="P161" s="225"/>
+      <c r="Q161" s="225"/>
+      <c r="R161" s="226"/>
       <c r="S161" s="180"/>
     </row>
     <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" s="46">
         <v>4</v>
       </c>
-      <c r="B162" s="260" t="s">
+      <c r="B162" s="271" t="s">
         <v>125</v>
       </c>
-      <c r="C162" s="215"/>
-      <c r="D162" s="215"/>
-      <c r="E162" s="216"/>
-      <c r="F162" s="258" t="s">
-        <v>154</v>
-      </c>
-      <c r="G162" s="259"/>
-      <c r="H162" s="219"/>
-      <c r="I162" s="260" t="s">
-        <v>155</v>
-      </c>
-      <c r="J162" s="215"/>
-      <c r="K162" s="215"/>
-      <c r="L162" s="215"/>
-      <c r="M162" s="215"/>
-      <c r="N162" s="215"/>
-      <c r="O162" s="215"/>
-      <c r="P162" s="215"/>
-      <c r="Q162" s="215"/>
-      <c r="R162" s="216"/>
+      <c r="C162" s="225"/>
+      <c r="D162" s="225"/>
+      <c r="E162" s="226"/>
+      <c r="F162" s="269" t="s">
+        <v>145</v>
+      </c>
+      <c r="G162" s="270"/>
+      <c r="H162" s="244"/>
+      <c r="I162" s="271" t="s">
+        <v>146</v>
+      </c>
+      <c r="J162" s="225"/>
+      <c r="K162" s="225"/>
+      <c r="L162" s="225"/>
+      <c r="M162" s="225"/>
+      <c r="N162" s="225"/>
+      <c r="O162" s="225"/>
+      <c r="P162" s="225"/>
+      <c r="Q162" s="225"/>
+      <c r="R162" s="226"/>
       <c r="S162" s="180"/>
     </row>
     <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" s="46">
         <v>5</v>
       </c>
-      <c r="B163" s="260" t="s">
+      <c r="B163" s="271" t="s">
         <v>126</v>
       </c>
-      <c r="C163" s="215"/>
-      <c r="D163" s="215"/>
-      <c r="E163" s="216"/>
-      <c r="F163" s="258" t="s">
-        <v>154</v>
-      </c>
-      <c r="G163" s="259"/>
-      <c r="H163" s="219"/>
-      <c r="I163" s="260" t="s">
-        <v>156</v>
-      </c>
-      <c r="J163" s="215"/>
-      <c r="K163" s="215"/>
-      <c r="L163" s="215"/>
-      <c r="M163" s="215"/>
-      <c r="N163" s="215"/>
-      <c r="O163" s="215"/>
-      <c r="P163" s="215"/>
-      <c r="Q163" s="215"/>
-      <c r="R163" s="216"/>
+      <c r="C163" s="225"/>
+      <c r="D163" s="225"/>
+      <c r="E163" s="226"/>
+      <c r="F163" s="269" t="s">
+        <v>145</v>
+      </c>
+      <c r="G163" s="270"/>
+      <c r="H163" s="244"/>
+      <c r="I163" s="271" t="s">
+        <v>147</v>
+      </c>
+      <c r="J163" s="225"/>
+      <c r="K163" s="225"/>
+      <c r="L163" s="225"/>
+      <c r="M163" s="225"/>
+      <c r="N163" s="225"/>
+      <c r="O163" s="225"/>
+      <c r="P163" s="225"/>
+      <c r="Q163" s="225"/>
+      <c r="R163" s="226"/>
     </row>
     <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" s="46">
         <v>6</v>
       </c>
-      <c r="B164" s="260" t="s">
+      <c r="B164" s="271" t="s">
         <v>127</v>
       </c>
-      <c r="C164" s="215"/>
-      <c r="D164" s="215"/>
-      <c r="E164" s="216"/>
-      <c r="F164" s="258" t="s">
-        <v>154</v>
-      </c>
-      <c r="G164" s="259"/>
-      <c r="H164" s="219"/>
-      <c r="I164" s="260"/>
-      <c r="J164" s="215"/>
-      <c r="K164" s="215"/>
-      <c r="L164" s="215"/>
-      <c r="M164" s="215"/>
-      <c r="N164" s="215"/>
-      <c r="O164" s="215"/>
-      <c r="P164" s="215"/>
-      <c r="Q164" s="215"/>
-      <c r="R164" s="216"/>
+      <c r="C164" s="225"/>
+      <c r="D164" s="225"/>
+      <c r="E164" s="226"/>
+      <c r="F164" s="269" t="s">
+        <v>145</v>
+      </c>
+      <c r="G164" s="270"/>
+      <c r="H164" s="244"/>
+      <c r="I164" s="271"/>
+      <c r="J164" s="225"/>
+      <c r="K164" s="225"/>
+      <c r="L164" s="225"/>
+      <c r="M164" s="225"/>
+      <c r="N164" s="225"/>
+      <c r="O164" s="225"/>
+      <c r="P164" s="225"/>
+      <c r="Q164" s="225"/>
+      <c r="R164" s="226"/>
     </row>
     <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" s="46">
         <v>7</v>
       </c>
-      <c r="B165" s="260" t="str">
-        <f>IFERROR("Total number of flights handled in Week ("&amp;R5-1&amp;")",""-"")</f>
-        <v>Total number of flights handled in Week (-1)</v>
-      </c>
-      <c r="C165" s="215"/>
-      <c r="D165" s="215"/>
-      <c r="E165" s="216"/>
-      <c r="F165" s="281">
+      <c r="B165" s="271"/>
+      <c r="C165" s="225"/>
+      <c r="D165" s="225"/>
+      <c r="E165" s="226"/>
+      <c r="F165" s="276">
         <v>349</v>
       </c>
-      <c r="G165" s="259"/>
-      <c r="H165" s="219"/>
-      <c r="I165" s="260" t="s">
-        <v>157</v>
-      </c>
-      <c r="J165" s="215"/>
-      <c r="K165" s="215"/>
-      <c r="L165" s="215"/>
-      <c r="M165" s="215"/>
-      <c r="N165" s="215"/>
-      <c r="O165" s="215"/>
-      <c r="P165" s="215"/>
-      <c r="Q165" s="215"/>
-      <c r="R165" s="216"/>
+      <c r="G165" s="270"/>
+      <c r="H165" s="244"/>
+      <c r="I165" s="271" t="s">
+        <v>148</v>
+      </c>
+      <c r="J165" s="225"/>
+      <c r="K165" s="225"/>
+      <c r="L165" s="225"/>
+      <c r="M165" s="225"/>
+      <c r="N165" s="225"/>
+      <c r="O165" s="225"/>
+      <c r="P165" s="225"/>
+      <c r="Q165" s="225"/>
+      <c r="R165" s="226"/>
     </row>
     <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" s="46">
         <v>8</v>
       </c>
-      <c r="B166" s="260" t="str">
-        <f>IFERROR("Total number of flights handled in Week ("&amp;R5&amp;")",""-"")</f>
-        <v>Total number of flights handled in Week ()</v>
-      </c>
-      <c r="C166" s="215"/>
-      <c r="D166" s="215"/>
-      <c r="E166" s="216"/>
-      <c r="F166" s="281">
+      <c r="B166" s="271"/>
+      <c r="C166" s="225"/>
+      <c r="D166" s="225"/>
+      <c r="E166" s="226"/>
+      <c r="F166" s="276">
         <v>356</v>
       </c>
-      <c r="G166" s="259"/>
-      <c r="H166" s="219"/>
-      <c r="I166" s="260" t="s">
-        <v>157</v>
-      </c>
-      <c r="J166" s="215"/>
-      <c r="K166" s="215"/>
-      <c r="L166" s="215"/>
-      <c r="M166" s="215"/>
-      <c r="N166" s="215"/>
-      <c r="O166" s="215"/>
-      <c r="P166" s="215"/>
-      <c r="Q166" s="215"/>
-      <c r="R166" s="216"/>
+      <c r="G166" s="270"/>
+      <c r="H166" s="244"/>
+      <c r="I166" s="271" t="s">
+        <v>148</v>
+      </c>
+      <c r="J166" s="225"/>
+      <c r="K166" s="225"/>
+      <c r="L166" s="225"/>
+      <c r="M166" s="225"/>
+      <c r="N166" s="225"/>
+      <c r="O166" s="225"/>
+      <c r="P166" s="225"/>
+      <c r="Q166" s="225"/>
+      <c r="R166" s="226"/>
     </row>
     <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" s="46">
         <v>9</v>
       </c>
-      <c r="B167" s="260" t="s">
+      <c r="B167" s="271" t="s">
         <v>128</v>
       </c>
-      <c r="C167" s="215"/>
-      <c r="D167" s="215"/>
-      <c r="E167" s="216"/>
-      <c r="F167" s="281">
-        <f>IFERROR(ABS(F165-F166),"-")</f>
-        <v>7</v>
-      </c>
-      <c r="G167" s="259"/>
-      <c r="H167" s="219"/>
-      <c r="I167" s="263" t="str">
-        <f>IFERROR(
-  IF(F166 - F165 &lt; 0,
-     "Decrease in flight frequency this week",
-     IF(F166 - F165 &gt; 0,
-        "Increase in flight frequency this week",
-        "Flight Frequency remains same"
-     )
-  ),
-  "-"
-)</f>
-        <v>Increase in flight frequency this week</v>
-      </c>
-      <c r="J167" s="215"/>
-      <c r="K167" s="215"/>
-      <c r="L167" s="215"/>
-      <c r="M167" s="215"/>
-      <c r="N167" s="215"/>
-      <c r="O167" s="215"/>
-      <c r="P167" s="215"/>
-      <c r="Q167" s="215"/>
-      <c r="R167" s="216"/>
+      <c r="C167" s="225"/>
+      <c r="D167" s="225"/>
+      <c r="E167" s="226"/>
+      <c r="F167" s="276"/>
+      <c r="G167" s="270"/>
+      <c r="H167" s="244"/>
+      <c r="I167" s="274"/>
+      <c r="J167" s="225"/>
+      <c r="K167" s="225"/>
+      <c r="L167" s="225"/>
+      <c r="M167" s="225"/>
+      <c r="N167" s="225"/>
+      <c r="O167" s="225"/>
+      <c r="P167" s="225"/>
+      <c r="Q167" s="225"/>
+      <c r="R167" s="226"/>
     </row>
     <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" s="46">
         <v>10</v>
       </c>
-      <c r="B168" s="260" t="str">
-        <f>IFERROR(
-  "Reason for the change in fuel consumption: " &amp;
-  IF(F166 - F165 &lt; 0,
-     "Low refilling requirement and flight frequency decreases (" &amp; ABS(F166 - F165) &amp; " less flights)",
-     "Low refilling requirement and flight frequency increases (" &amp; ABS(F166 - F165) &amp; " more flights)"
-  ),
-  "-"
-)</f>
-        <v>Reason for the change in fuel consumption: Low refilling requirement and flight frequency increases (7 more flights)</v>
-      </c>
-      <c r="C168" s="215"/>
-      <c r="D168" s="215"/>
-      <c r="E168" s="215"/>
-      <c r="F168" s="215"/>
-      <c r="G168" s="215"/>
-      <c r="H168" s="215"/>
-      <c r="I168" s="215"/>
-      <c r="J168" s="215"/>
-      <c r="K168" s="215"/>
-      <c r="L168" s="215"/>
-      <c r="M168" s="215"/>
-      <c r="N168" s="215"/>
-      <c r="O168" s="215"/>
-      <c r="P168" s="215"/>
-      <c r="Q168" s="215"/>
-      <c r="R168" s="216"/>
+      <c r="B168" s="271"/>
+      <c r="C168" s="225"/>
+      <c r="D168" s="225"/>
+      <c r="E168" s="225"/>
+      <c r="F168" s="225"/>
+      <c r="G168" s="225"/>
+      <c r="H168" s="225"/>
+      <c r="I168" s="225"/>
+      <c r="J168" s="225"/>
+      <c r="K168" s="225"/>
+      <c r="L168" s="225"/>
+      <c r="M168" s="225"/>
+      <c r="N168" s="225"/>
+      <c r="O168" s="225"/>
+      <c r="P168" s="225"/>
+      <c r="Q168" s="225"/>
+      <c r="R168" s="226"/>
     </row>
     <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" s="189" t="s">
         <v>129</v>
       </c>
-      <c r="B169" s="257" t="s">
+      <c r="B169" s="275" t="s">
         <v>130</v>
       </c>
-      <c r="C169" s="215"/>
-      <c r="D169" s="215"/>
-      <c r="E169" s="215"/>
-      <c r="F169" s="215"/>
-      <c r="G169" s="215"/>
-      <c r="H169" s="215"/>
-      <c r="I169" s="215"/>
-      <c r="J169" s="215"/>
-      <c r="K169" s="215"/>
-      <c r="L169" s="215"/>
-      <c r="M169" s="215"/>
-      <c r="N169" s="215"/>
-      <c r="O169" s="215"/>
-      <c r="P169" s="215"/>
-      <c r="Q169" s="215"/>
-      <c r="R169" s="216"/>
+      <c r="C169" s="225"/>
+      <c r="D169" s="225"/>
+      <c r="E169" s="225"/>
+      <c r="F169" s="225"/>
+      <c r="G169" s="225"/>
+      <c r="H169" s="225"/>
+      <c r="I169" s="225"/>
+      <c r="J169" s="225"/>
+      <c r="K169" s="225"/>
+      <c r="L169" s="225"/>
+      <c r="M169" s="225"/>
+      <c r="N169" s="225"/>
+      <c r="O169" s="225"/>
+      <c r="P169" s="225"/>
+      <c r="Q169" s="225"/>
+      <c r="R169" s="226"/>
     </row>
     <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" s="187">
         <v>1</v>
       </c>
-      <c r="B170" s="260" t="str">
-        <f>IFERROR("Total cost of diesel issued in Week ("&amp;R5-1&amp;")",""-"")</f>
-        <v>Total cost of diesel issued in Week (-1)</v>
-      </c>
-      <c r="C170" s="215"/>
-      <c r="D170" s="215"/>
-      <c r="E170" s="216"/>
-      <c r="F170" s="258" t="str">
-        <f t="array" aca="1" ref="F170" ca="1">IFERROR(INDIRECT("'" &amp; R5-1 &amp; "'!R155"),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="G170" s="259"/>
-      <c r="H170" s="219"/>
-      <c r="I170" s="226"/>
-      <c r="J170" s="215"/>
-      <c r="K170" s="215"/>
-      <c r="L170" s="215"/>
-      <c r="M170" s="215"/>
-      <c r="N170" s="215"/>
-      <c r="O170" s="215"/>
-      <c r="P170" s="215"/>
-      <c r="Q170" s="215"/>
-      <c r="R170" s="216"/>
+      <c r="B170" s="271"/>
+      <c r="C170" s="225"/>
+      <c r="D170" s="225"/>
+      <c r="E170" s="226"/>
+      <c r="F170" s="269"/>
+      <c r="G170" s="270"/>
+      <c r="H170" s="244"/>
+      <c r="I170" s="232"/>
+      <c r="J170" s="225"/>
+      <c r="K170" s="225"/>
+      <c r="L170" s="225"/>
+      <c r="M170" s="225"/>
+      <c r="N170" s="225"/>
+      <c r="O170" s="225"/>
+      <c r="P170" s="225"/>
+      <c r="Q170" s="225"/>
+      <c r="R170" s="226"/>
     </row>
     <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" s="187">
         <v>2</v>
       </c>
-      <c r="B171" s="260" t="str">
-        <f>IFERROR("Total cost of diesel issued in Week ("&amp;R5&amp;")",""-"")</f>
-        <v>Total cost of diesel issued in Week ()</v>
-      </c>
-      <c r="C171" s="215"/>
-      <c r="D171" s="215"/>
-      <c r="E171" s="216"/>
-      <c r="F171" s="258" t="str">
-        <f t="array" aca="1" ref="F171" ca="1">IFERROR(INDIRECT("'" &amp; R5&amp; "'!R155"),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="G171" s="259"/>
-      <c r="H171" s="219"/>
-      <c r="I171" s="262"/>
-      <c r="J171" s="215"/>
-      <c r="K171" s="215"/>
-      <c r="L171" s="215"/>
-      <c r="M171" s="215"/>
-      <c r="N171" s="215"/>
-      <c r="O171" s="215"/>
-      <c r="P171" s="215"/>
-      <c r="Q171" s="215"/>
-      <c r="R171" s="216"/>
+      <c r="B171" s="271"/>
+      <c r="C171" s="225"/>
+      <c r="D171" s="225"/>
+      <c r="E171" s="226"/>
+      <c r="F171" s="269"/>
+      <c r="G171" s="270"/>
+      <c r="H171" s="244"/>
+      <c r="I171" s="273"/>
+      <c r="J171" s="225"/>
+      <c r="K171" s="225"/>
+      <c r="L171" s="225"/>
+      <c r="M171" s="225"/>
+      <c r="N171" s="225"/>
+      <c r="O171" s="225"/>
+      <c r="P171" s="225"/>
+      <c r="Q171" s="225"/>
+      <c r="R171" s="226"/>
     </row>
     <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" s="187">
         <v>3</v>
       </c>
-      <c r="B172" s="260" t="s">
+      <c r="B172" s="271" t="s">
         <v>131</v>
       </c>
-      <c r="C172" s="215"/>
-      <c r="D172" s="215"/>
-      <c r="E172" s="216"/>
-      <c r="F172" s="258">
-        <f ca="1">IFERROR(F170-F171,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G172" s="259"/>
-      <c r="H172" s="219"/>
-      <c r="I172" s="263" t="str">
-        <f ca="1">IFERROR(
+      <c r="C172" s="225"/>
+      <c r="D172" s="225"/>
+      <c r="E172" s="226"/>
+      <c r="F172" s="269"/>
+      <c r="G172" s="270"/>
+      <c r="H172" s="244"/>
+      <c r="I172" s="274" t="str">
+        <f>IFERROR(
   IF(F171-F170 &lt; 0,
      "Decrease in total cost this week",
     " Increase in total cost this week"
   ),
   "-"
 )</f>
-        <v>-</v>
-      </c>
-      <c r="J172" s="215"/>
-      <c r="K172" s="215"/>
-      <c r="L172" s="215"/>
-      <c r="M172" s="215"/>
-      <c r="N172" s="215"/>
-      <c r="O172" s="215"/>
-      <c r="P172" s="215"/>
-      <c r="Q172" s="215"/>
-      <c r="R172" s="216"/>
+        <v xml:space="preserve"> Increase in total cost this week</v>
+      </c>
+      <c r="J172" s="225"/>
+      <c r="K172" s="225"/>
+      <c r="L172" s="225"/>
+      <c r="M172" s="225"/>
+      <c r="N172" s="225"/>
+      <c r="O172" s="225"/>
+      <c r="P172" s="225"/>
+      <c r="Q172" s="225"/>
+      <c r="R172" s="226"/>
     </row>
     <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" s="187">
@@ -14032,145 +14028,85 @@
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
       <c r="E173" s="193"/>
-      <c r="F173" s="258" t="str">
+      <c r="F173" s="269" t="str">
         <f t="array" aca="1" ref="F173" ca="1">IFERROR(INDIRECT("'" &amp; R5-1 &amp; "'!F173") - R155, "-")</f>
         <v>-</v>
       </c>
-      <c r="G173" s="259"/>
-      <c r="H173" s="219"/>
-      <c r="I173" s="260" t="s">
-        <v>158</v>
-      </c>
-      <c r="J173" s="215"/>
-      <c r="K173" s="215"/>
-      <c r="L173" s="215"/>
-      <c r="M173" s="215"/>
-      <c r="N173" s="215"/>
-      <c r="O173" s="215"/>
-      <c r="P173" s="215"/>
-      <c r="Q173" s="215"/>
-      <c r="R173" s="216"/>
+      <c r="G173" s="270"/>
+      <c r="H173" s="244"/>
+      <c r="I173" s="271" t="s">
+        <v>149</v>
+      </c>
+      <c r="J173" s="225"/>
+      <c r="K173" s="225"/>
+      <c r="L173" s="225"/>
+      <c r="M173" s="225"/>
+      <c r="N173" s="225"/>
+      <c r="O173" s="225"/>
+      <c r="P173" s="225"/>
+      <c r="Q173" s="225"/>
+      <c r="R173" s="226"/>
     </row>
     <row r="174" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="187">
         <v>5</v>
       </c>
-      <c r="B174" s="261" t="s">
-        <v>161</v>
-      </c>
-      <c r="C174" s="215"/>
-      <c r="D174" s="215"/>
-      <c r="E174" s="215"/>
-      <c r="F174" s="215"/>
-      <c r="G174" s="215"/>
-      <c r="H174" s="215"/>
-      <c r="I174" s="215"/>
-      <c r="J174" s="215"/>
-      <c r="K174" s="215"/>
-      <c r="L174" s="215"/>
-      <c r="M174" s="215"/>
-      <c r="N174" s="215"/>
-      <c r="O174" s="215"/>
-      <c r="P174" s="215"/>
-      <c r="Q174" s="215"/>
-      <c r="R174" s="216"/>
+      <c r="B174" s="272"/>
+      <c r="C174" s="225"/>
+      <c r="D174" s="225"/>
+      <c r="E174" s="225"/>
+      <c r="F174" s="225"/>
+      <c r="G174" s="225"/>
+      <c r="H174" s="225"/>
+      <c r="I174" s="225"/>
+      <c r="J174" s="225"/>
+      <c r="K174" s="225"/>
+      <c r="L174" s="225"/>
+      <c r="M174" s="225"/>
+      <c r="N174" s="225"/>
+      <c r="O174" s="225"/>
+      <c r="P174" s="225"/>
+      <c r="Q174" s="225"/>
+      <c r="R174" s="226"/>
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A189" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="A189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
       <c r="E189" s="194"/>
       <c r="F189" s="1"/>
       <c r="G189" s="194"/>
       <c r="H189" s="1"/>
-      <c r="I189" s="194" t="s">
-        <v>134</v>
-      </c>
+      <c r="I189" s="194"/>
       <c r="J189" s="1"/>
       <c r="K189" s="194"/>
       <c r="L189" s="1"/>
       <c r="M189" s="195"/>
       <c r="N189" s="1"/>
       <c r="O189" s="1"/>
-      <c r="P189" s="181" t="s">
-        <v>135</v>
-      </c>
+      <c r="P189" s="181"/>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A190" s="34" t="s">
-        <v>136</v>
-      </c>
       <c r="E190" s="196"/>
       <c r="G190" s="196"/>
-      <c r="I190" s="196" t="s">
-        <v>137</v>
-      </c>
+      <c r="I190" s="196"/>
       <c r="K190" s="196"/>
       <c r="M190" s="195"/>
-      <c r="P190" s="181" t="s">
-        <v>138</v>
-      </c>
+      <c r="P190" s="181"/>
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A191" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="I191" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="P191" s="181" t="s">
-        <v>141</v>
-      </c>
+      <c r="P191" s="181"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="F173:H173"/>
-    <mergeCell ref="I173:R173"/>
-    <mergeCell ref="B174:R174"/>
-    <mergeCell ref="B171:E171"/>
-    <mergeCell ref="F171:H171"/>
-    <mergeCell ref="I171:R171"/>
-    <mergeCell ref="B172:E172"/>
-    <mergeCell ref="F172:H172"/>
-    <mergeCell ref="I172:R172"/>
-    <mergeCell ref="B168:R168"/>
-    <mergeCell ref="B169:R169"/>
-    <mergeCell ref="B170:E170"/>
-    <mergeCell ref="F170:H170"/>
-    <mergeCell ref="I170:R170"/>
-    <mergeCell ref="B166:E166"/>
-    <mergeCell ref="F166:H166"/>
-    <mergeCell ref="I166:R166"/>
-    <mergeCell ref="B167:E167"/>
-    <mergeCell ref="F167:H167"/>
-    <mergeCell ref="I167:R167"/>
-    <mergeCell ref="B164:E164"/>
-    <mergeCell ref="F164:H164"/>
-    <mergeCell ref="I164:R164"/>
-    <mergeCell ref="B165:E165"/>
-    <mergeCell ref="F165:H165"/>
-    <mergeCell ref="I165:R165"/>
-    <mergeCell ref="B162:E162"/>
-    <mergeCell ref="F162:H162"/>
-    <mergeCell ref="I162:R162"/>
-    <mergeCell ref="B163:E163"/>
-    <mergeCell ref="F163:H163"/>
-    <mergeCell ref="I163:R163"/>
-    <mergeCell ref="B160:E160"/>
-    <mergeCell ref="F160:H160"/>
-    <mergeCell ref="I160:R160"/>
-    <mergeCell ref="B161:E161"/>
-    <mergeCell ref="F161:H161"/>
-    <mergeCell ref="I161:R161"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="A157:Q157"/>
-    <mergeCell ref="B158:R158"/>
-    <mergeCell ref="B159:E159"/>
-    <mergeCell ref="F159:H159"/>
-    <mergeCell ref="I159:R159"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="A153:P153"/>
     <mergeCell ref="A154:B154"/>
     <mergeCell ref="A1:R1"/>
@@ -14187,16 +14123,997 @@
     <mergeCell ref="O7:P8"/>
     <mergeCell ref="Q7:Q10"/>
     <mergeCell ref="R7:R10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="A157:Q157"/>
+    <mergeCell ref="B158:R158"/>
+    <mergeCell ref="B159:E159"/>
+    <mergeCell ref="F159:H159"/>
+    <mergeCell ref="I159:R159"/>
+    <mergeCell ref="B160:E160"/>
+    <mergeCell ref="F160:H160"/>
+    <mergeCell ref="I160:R160"/>
+    <mergeCell ref="B161:E161"/>
+    <mergeCell ref="F161:H161"/>
+    <mergeCell ref="I161:R161"/>
+    <mergeCell ref="B162:E162"/>
+    <mergeCell ref="F162:H162"/>
+    <mergeCell ref="I162:R162"/>
+    <mergeCell ref="B163:E163"/>
+    <mergeCell ref="F163:H163"/>
+    <mergeCell ref="I163:R163"/>
+    <mergeCell ref="B164:E164"/>
+    <mergeCell ref="F164:H164"/>
+    <mergeCell ref="I164:R164"/>
+    <mergeCell ref="B165:E165"/>
+    <mergeCell ref="F165:H165"/>
+    <mergeCell ref="I165:R165"/>
+    <mergeCell ref="B166:E166"/>
+    <mergeCell ref="F166:H166"/>
+    <mergeCell ref="I166:R166"/>
+    <mergeCell ref="B167:E167"/>
+    <mergeCell ref="F167:H167"/>
+    <mergeCell ref="I167:R167"/>
+    <mergeCell ref="B168:R168"/>
+    <mergeCell ref="B169:R169"/>
+    <mergeCell ref="B170:E170"/>
+    <mergeCell ref="F170:H170"/>
+    <mergeCell ref="I170:R170"/>
+    <mergeCell ref="F173:H173"/>
+    <mergeCell ref="I173:R173"/>
+    <mergeCell ref="B174:R174"/>
+    <mergeCell ref="B171:E171"/>
+    <mergeCell ref="F171:H171"/>
+    <mergeCell ref="I171:R171"/>
+    <mergeCell ref="B172:E172"/>
+    <mergeCell ref="F172:H172"/>
+    <mergeCell ref="I172:R172"/>
+  </mergeCells>
+  <pageMargins left="0.24" right="0.16" top="0.49" bottom="0.2" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83219E9D-79C7-4B40-B1CF-7509B7FF5A6B}">
+  <dimension ref="A6:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" style="293" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" style="293" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="293" customWidth="1"/>
+    <col min="4" max="4" width="19" style="293" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="293" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="293"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="294"/>
+      <c r="D6" s="295" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="296"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="297"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="293" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8" s="293" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="295"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="295" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="293" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="295"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="290" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="283"/>
+      <c r="C11" s="283"/>
+      <c r="D11" s="283"/>
+      <c r="E11" s="283"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="298" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="299"/>
+      <c r="D13" s="300"/>
+      <c r="E13" s="301"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="302"/>
+      <c r="C14" s="303"/>
+      <c r="D14" s="304"/>
+      <c r="E14" s="305"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="306" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="309" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" s="309" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="309" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="309" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="310">
+        <v>1</v>
+      </c>
+      <c r="B16" s="311"/>
+      <c r="C16" s="310"/>
+      <c r="D16" s="310"/>
+      <c r="E16" s="310"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="310">
+        <v>2</v>
+      </c>
+      <c r="B17" s="311"/>
+      <c r="C17" s="310"/>
+      <c r="D17" s="310"/>
+      <c r="E17" s="310"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="310">
+        <v>3</v>
+      </c>
+      <c r="B18" s="311"/>
+      <c r="C18" s="310"/>
+      <c r="D18" s="310"/>
+      <c r="E18" s="310"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="310">
+        <v>4</v>
+      </c>
+      <c r="B19" s="311"/>
+      <c r="C19" s="310"/>
+      <c r="D19" s="310"/>
+      <c r="E19" s="310"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="310">
+        <v>5</v>
+      </c>
+      <c r="B20" s="311"/>
+      <c r="C20" s="310"/>
+      <c r="D20" s="310"/>
+      <c r="E20" s="310"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="310">
+        <v>6</v>
+      </c>
+      <c r="B21" s="311"/>
+      <c r="C21" s="310"/>
+      <c r="D21" s="310"/>
+      <c r="E21" s="310"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="310">
+        <v>7</v>
+      </c>
+      <c r="B22" s="311"/>
+      <c r="C22" s="310"/>
+      <c r="D22" s="310"/>
+      <c r="E22" s="310"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="310">
+        <v>8</v>
+      </c>
+      <c r="B23" s="311"/>
+      <c r="C23" s="310"/>
+      <c r="D23" s="310"/>
+      <c r="E23" s="310"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="310">
+        <v>9</v>
+      </c>
+      <c r="B24" s="311"/>
+      <c r="C24" s="310"/>
+      <c r="D24" s="310"/>
+      <c r="E24" s="310"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="310">
+        <v>10</v>
+      </c>
+      <c r="B25" s="311"/>
+      <c r="C25" s="310"/>
+      <c r="D25" s="310"/>
+      <c r="E25" s="310"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="310">
+        <v>11</v>
+      </c>
+      <c r="B26" s="311"/>
+      <c r="C26" s="310"/>
+      <c r="D26" s="310"/>
+      <c r="E26" s="310"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="310">
+        <v>12</v>
+      </c>
+      <c r="B27" s="311"/>
+      <c r="C27" s="310"/>
+      <c r="D27" s="310"/>
+      <c r="E27" s="310"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="310">
+        <v>13</v>
+      </c>
+      <c r="B28" s="311"/>
+      <c r="C28" s="310"/>
+      <c r="D28" s="310"/>
+      <c r="E28" s="310"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="310">
+        <v>14</v>
+      </c>
+      <c r="B29" s="311"/>
+      <c r="C29" s="310"/>
+      <c r="D29" s="310"/>
+      <c r="E29" s="310"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="310">
+        <v>15</v>
+      </c>
+      <c r="B30" s="311"/>
+      <c r="C30" s="310"/>
+      <c r="D30" s="310"/>
+      <c r="E30" s="310"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="310">
+        <v>16</v>
+      </c>
+      <c r="B31" s="311"/>
+      <c r="C31" s="310"/>
+      <c r="D31" s="310"/>
+      <c r="E31" s="310"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="310">
+        <v>17</v>
+      </c>
+      <c r="B32" s="311"/>
+      <c r="C32" s="310"/>
+      <c r="D32" s="310"/>
+      <c r="E32" s="310"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="307"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="292"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="308"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="307"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F44584-3A0B-4F85-A637-D8D008062A45}">
+  <dimension ref="A1:S30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="176" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="34" customWidth="1"/>
+    <col min="4" max="4" width="9" style="34" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="34" customWidth="1"/>
+    <col min="6" max="6" width="9" style="34" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="34" customWidth="1"/>
+    <col min="8" max="8" width="9" style="34" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="34" customWidth="1"/>
+    <col min="10" max="10" width="9" style="34" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="34" customWidth="1"/>
+    <col min="12" max="12" width="9" style="34" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" style="34" customWidth="1"/>
+    <col min="14" max="14" width="9" style="34" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="34" customWidth="1"/>
+    <col min="16" max="16" width="9" style="34" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="34" customWidth="1"/>
+    <col min="18" max="18" width="15" style="34" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="34"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="282" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="282"/>
+      <c r="C1" s="283"/>
+      <c r="D1" s="283"/>
+      <c r="E1" s="283"/>
+      <c r="F1" s="283"/>
+      <c r="G1" s="283"/>
+      <c r="H1" s="283"/>
+      <c r="I1" s="283"/>
+      <c r="J1" s="283"/>
+      <c r="K1" s="283"/>
+      <c r="L1" s="283"/>
+      <c r="M1" s="283"/>
+      <c r="N1" s="283"/>
+      <c r="O1" s="283"/>
+      <c r="P1" s="283"/>
+      <c r="Q1" s="283"/>
+      <c r="R1" s="283"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="282" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="282"/>
+      <c r="C2" s="283"/>
+      <c r="D2" s="283"/>
+      <c r="E2" s="283"/>
+      <c r="F2" s="283"/>
+      <c r="G2" s="283"/>
+      <c r="H2" s="283"/>
+      <c r="I2" s="283"/>
+      <c r="J2" s="283"/>
+      <c r="K2" s="283"/>
+      <c r="L2" s="283"/>
+      <c r="M2" s="283"/>
+      <c r="N2" s="283"/>
+      <c r="O2" s="283"/>
+      <c r="P2" s="283"/>
+      <c r="Q2" s="283"/>
+      <c r="R2" s="283"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="291" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="282"/>
+      <c r="C3" s="283"/>
+      <c r="D3" s="283"/>
+      <c r="E3" s="283"/>
+      <c r="F3" s="283"/>
+      <c r="G3" s="283"/>
+      <c r="H3" s="283"/>
+      <c r="I3" s="283"/>
+      <c r="J3" s="283"/>
+      <c r="K3" s="283"/>
+      <c r="L3" s="283"/>
+      <c r="M3" s="283"/>
+      <c r="N3" s="283"/>
+      <c r="O3" s="283"/>
+      <c r="P3" s="283"/>
+      <c r="Q3" s="283"/>
+      <c r="R3" s="283"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="177"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="179"/>
+      <c r="C5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="N5" s="180"/>
+      <c r="Q5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R5" s="201"/>
+      <c r="S5" s="202"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="180" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="N6" s="177"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R6" s="203"/>
+    </row>
+    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="286" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="234"/>
+      <c r="C7" s="277"/>
+      <c r="D7" s="234"/>
+      <c r="E7" s="277"/>
+      <c r="F7" s="234"/>
+      <c r="G7" s="277"/>
+      <c r="H7" s="234"/>
+      <c r="I7" s="277"/>
+      <c r="J7" s="234"/>
+      <c r="K7" s="277"/>
+      <c r="L7" s="234"/>
+      <c r="M7" s="277"/>
+      <c r="N7" s="234"/>
+      <c r="O7" s="277"/>
+      <c r="P7" s="234"/>
+      <c r="Q7" s="277" t="s">
+        <v>114</v>
+      </c>
+      <c r="R7" s="277" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="287"/>
+      <c r="B8" s="244"/>
+      <c r="C8" s="287"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="287"/>
+      <c r="F8" s="244"/>
+      <c r="G8" s="287"/>
+      <c r="H8" s="244"/>
+      <c r="I8" s="287"/>
+      <c r="J8" s="244"/>
+      <c r="K8" s="287"/>
+      <c r="L8" s="244"/>
+      <c r="M8" s="287"/>
+      <c r="N8" s="244"/>
+      <c r="O8" s="287"/>
+      <c r="P8" s="244"/>
+      <c r="Q8" s="288"/>
+      <c r="R8" s="288"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="286" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="226"/>
+      <c r="C9" s="277"/>
+      <c r="D9" s="226"/>
+      <c r="E9" s="277"/>
+      <c r="F9" s="226"/>
+      <c r="G9" s="277"/>
+      <c r="H9" s="226"/>
+      <c r="I9" s="277"/>
+      <c r="J9" s="226"/>
+      <c r="K9" s="277"/>
+      <c r="L9" s="226"/>
+      <c r="M9" s="277"/>
+      <c r="N9" s="226"/>
+      <c r="O9" s="277"/>
+      <c r="P9" s="226"/>
+      <c r="Q9" s="289"/>
+      <c r="R9" s="289"/>
+    </row>
+    <row r="10" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="183" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="184" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="185" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="185" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="185" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="185" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="185" t="s">
+        <v>118</v>
+      </c>
+      <c r="I10" s="185" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="185" t="s">
+        <v>118</v>
+      </c>
+      <c r="K10" s="185" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="185" t="s">
+        <v>118</v>
+      </c>
+      <c r="M10" s="185" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="185" t="s">
+        <v>118</v>
+      </c>
+      <c r="O10" s="185" t="s">
+        <v>47</v>
+      </c>
+      <c r="P10" s="185" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q10" s="183"/>
+      <c r="R10" s="183"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="94">
+        <v>1</v>
+      </c>
+      <c r="B11" s="197">
+        <v>1214</v>
+      </c>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="204"/>
+      <c r="I11" s="187"/>
+      <c r="J11" s="187"/>
+      <c r="K11" s="187"/>
+      <c r="L11" s="187"/>
+      <c r="M11" s="187"/>
+      <c r="N11" s="187"/>
+      <c r="O11" s="187"/>
+      <c r="P11" s="187"/>
+      <c r="Q11" s="187"/>
+      <c r="R11" s="188"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="94">
+        <v>2</v>
+      </c>
+      <c r="B12" s="197">
+        <v>1219</v>
+      </c>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="187"/>
+      <c r="J12" s="187"/>
+      <c r="K12" s="187"/>
+      <c r="L12" s="187"/>
+      <c r="M12" s="187"/>
+      <c r="N12" s="187"/>
+      <c r="O12" s="187"/>
+      <c r="P12" s="187"/>
+      <c r="Q12" s="187"/>
+      <c r="R12" s="188"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="94">
+        <v>3</v>
+      </c>
+      <c r="B13" s="197">
+        <v>1223</v>
+      </c>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="187"/>
+      <c r="J13" s="187"/>
+      <c r="K13" s="187"/>
+      <c r="L13" s="187"/>
+      <c r="M13" s="187"/>
+      <c r="N13" s="187"/>
+      <c r="O13" s="187"/>
+      <c r="P13" s="187"/>
+      <c r="Q13" s="187"/>
+      <c r="R13" s="188"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="94">
+        <v>4</v>
+      </c>
+      <c r="B14" s="197">
+        <v>1225</v>
+      </c>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="204"/>
+      <c r="I14" s="187"/>
+      <c r="J14" s="187"/>
+      <c r="K14" s="187"/>
+      <c r="L14" s="187"/>
+      <c r="M14" s="187"/>
+      <c r="N14" s="187"/>
+      <c r="O14" s="187"/>
+      <c r="P14" s="187"/>
+      <c r="Q14" s="187"/>
+      <c r="R14" s="188"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="94">
+        <v>5</v>
+      </c>
+      <c r="B15" s="197">
+        <v>1226</v>
+      </c>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="204"/>
+      <c r="I15" s="187"/>
+      <c r="J15" s="187"/>
+      <c r="K15" s="187"/>
+      <c r="L15" s="187"/>
+      <c r="M15" s="187"/>
+      <c r="N15" s="187"/>
+      <c r="O15" s="187"/>
+      <c r="P15" s="187"/>
+      <c r="Q15" s="187"/>
+      <c r="R15" s="188"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="94">
+        <v>6</v>
+      </c>
+      <c r="B16" s="197">
+        <v>1227</v>
+      </c>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="204"/>
+      <c r="I16" s="187"/>
+      <c r="J16" s="187"/>
+      <c r="K16" s="187"/>
+      <c r="L16" s="187"/>
+      <c r="M16" s="187"/>
+      <c r="N16" s="187"/>
+      <c r="O16" s="187"/>
+      <c r="P16" s="187"/>
+      <c r="Q16" s="187"/>
+      <c r="R16" s="188"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="94">
+        <v>7</v>
+      </c>
+      <c r="B17" s="197">
+        <v>1228</v>
+      </c>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="94"/>
+      <c r="K17" s="94"/>
+      <c r="L17" s="94"/>
+      <c r="M17" s="94"/>
+      <c r="N17" s="94"/>
+      <c r="O17" s="94"/>
+      <c r="P17" s="94"/>
+      <c r="Q17" s="187"/>
+      <c r="R17" s="188"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="94">
+        <v>8</v>
+      </c>
+      <c r="B18" s="197">
+        <v>1239</v>
+      </c>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="94"/>
+      <c r="N18" s="94"/>
+      <c r="O18" s="94"/>
+      <c r="P18" s="94"/>
+      <c r="Q18" s="187"/>
+      <c r="R18" s="188"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="94">
+        <v>9</v>
+      </c>
+      <c r="B19" s="187" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" s="187"/>
+      <c r="D19" s="187"/>
+      <c r="E19" s="187"/>
+      <c r="F19" s="187"/>
+      <c r="G19" s="187"/>
+      <c r="H19" s="187"/>
+      <c r="I19" s="187"/>
+      <c r="J19" s="187"/>
+      <c r="K19" s="187"/>
+      <c r="L19" s="187"/>
+      <c r="M19" s="187"/>
+      <c r="N19" s="187"/>
+      <c r="O19" s="187"/>
+      <c r="P19" s="187"/>
+      <c r="Q19" s="187"/>
+      <c r="R19" s="188"/>
+    </row>
+    <row r="20" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="273" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" s="225"/>
+      <c r="C20" s="225"/>
+      <c r="D20" s="225"/>
+      <c r="E20" s="225"/>
+      <c r="F20" s="225"/>
+      <c r="G20" s="225"/>
+      <c r="H20" s="225"/>
+      <c r="I20" s="225"/>
+      <c r="J20" s="225"/>
+      <c r="K20" s="225"/>
+      <c r="L20" s="225"/>
+      <c r="M20" s="225"/>
+      <c r="N20" s="225"/>
+      <c r="O20" s="225"/>
+      <c r="P20" s="226"/>
+      <c r="Q20" s="189"/>
+      <c r="R20" s="205"/>
+    </row>
+    <row r="21" spans="1:19" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="277" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" s="226"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="94"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="94"/>
+      <c r="I21" s="94"/>
+      <c r="J21" s="94"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="94"/>
+      <c r="M21" s="94"/>
+      <c r="N21" s="94"/>
+      <c r="O21" s="94"/>
+      <c r="P21" s="94"/>
+      <c r="Q21" s="187"/>
+      <c r="R21" s="206"/>
+    </row>
+    <row r="22" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="277" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="226"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="94"/>
+      <c r="H22" s="94"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="94"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="94"/>
+      <c r="O22" s="94"/>
+      <c r="P22" s="94"/>
+      <c r="Q22" s="94"/>
+      <c r="R22" s="190"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="278"/>
+      <c r="C23" s="279"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="207"/>
+      <c r="B25" s="208"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="207"/>
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="Q26" s="181" t="s">
+        <v>158</v>
+      </c>
+      <c r="R26" s="181"/>
+      <c r="S26" s="181"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q27" s="181"/>
+      <c r="R27" s="181"/>
+      <c r="S27" s="181"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="34"/>
+      <c r="C30" s="176"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A20:P20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="O9:P9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A3:R3"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="I7:J8"/>
+    <mergeCell ref="K7:L8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="O7:P8"/>
+    <mergeCell ref="Q7:Q9"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>